<commit_message>
complete read excel test case Comment
</commit_message>
<xml_diff>
--- a/DienmayXANH-FunctionalTestExecution.xlsx
+++ b/DienmayXANH-FunctionalTestExecution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\test cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienMayXanh\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309B18EF-B80E-45BD-B3D7-A34CB555A4F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB330B5B-A026-4061-86DF-7E606AF15A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t>GUI &amp; FUNCTIONAL TEST CASES</t>
   </si>
@@ -91,6 +91,9 @@
     <t>0.1</t>
   </si>
   <si>
+    <t>Nhi Phan</t>
+  </si>
+  <si>
     <t>Drafts</t>
   </si>
   <si>
@@ -157,9 +160,42 @@
     <t>Note</t>
   </si>
   <si>
+    <t>TR-DMX-BL-01</t>
+  </si>
+  <si>
+    <t>Khách hàng có thể gửi bình luận thành công.</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
     <t>High</t>
   </si>
   <si>
+    <t>TR-DMX-BL-02</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo lỗi khi khách hàng không nhập nội dung</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>TR-DMX-BL-03</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo lỗi khi khách hàng không nhập họ tên</t>
+  </si>
+  <si>
+    <t>TR-DMX-BL-04</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo lỗi khi khách hàng nhập nội dung có số ký tự ít hơn 10</t>
+  </si>
+  <si>
+    <t>Boundary</t>
+  </si>
+  <si>
     <t>Test Case ID</t>
   </si>
   <si>
@@ -184,112 +220,127 @@
     <t>Functional TCs</t>
   </si>
   <si>
-    <t>Nhi Phan, Thanh Nhan</t>
-  </si>
-  <si>
-    <t>LooknFeel</t>
-  </si>
-  <si>
-    <t>TR-DMX-VLP-01</t>
-  </si>
-  <si>
-    <t>TR-DMX-VLP-02</t>
-  </si>
-  <si>
-    <t>TR-DMX-VLP-03</t>
-  </si>
-  <si>
-    <t>View list products</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị danh sách sản phẩm máy lọc nước theo giá thấp đến cao và giá cao đến thấp</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị danh sách tất cả sản phẩm máy lọc nước và danh sách máy lọc nước theo hãng</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-01</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-02</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-03</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-04</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-05</t>
-  </si>
-  <si>
-    <t>Test Cases for 'View list products' function</t>
-  </si>
-  <si>
-    <t>Xác nhận hệ thống hiển thị tất cả sản phẩm trong danh mục</t>
-  </si>
-  <si>
-    <t>Xác nhận hệ thống hiển thị tất cả sản phẩm trong danh mục theo hãng</t>
-  </si>
-  <si>
-    <t>Truy cập trang chủ điện máy xanh</t>
+    <t>TC-DMX-BL-01</t>
+  </si>
+  <si>
+    <t>Xác nhận rằng khách hàng có thể gửi bình luận.</t>
+  </si>
+  <si>
+    <t>Hệ thống phải hoạt động</t>
+  </si>
+  <si>
+    <t>Truy cập https://www.dienmayxanh.com/</t>
+  </si>
+  <si>
+    <t>Chọn mục Gửi góp ý, khiếu nại ở footer</t>
+  </si>
+  <si>
+    <t>Hiển thị trang Thông tin liên hệ, hỗ trợ, chăm sóc khách hàng của dienmayxanh.com</t>
+  </si>
+  <si>
+    <t>Nhập nội dung bình luận</t>
+  </si>
+  <si>
+    <t>Cho hỏi con e ném ổ khóa bể màn hình tivi 43inch hiệu TCL. Mới mua ạ</t>
+  </si>
+  <si>
+    <t>Nhập họ tên</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Tùng</t>
+  </si>
+  <si>
+    <t>Chọn gửi hình</t>
+  </si>
+  <si>
+    <t>Nhập email</t>
+  </si>
+  <si>
+    <t>tung@gmail.com</t>
+  </si>
+  <si>
+    <t>Chọn gửi</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-02</t>
+  </si>
+  <si>
+    <t>Xác nhận hệ thống hiển thị thông báo lỗi khi khách hàng không nhập nội dung</t>
+  </si>
+  <si>
+    <t>Không nội dung bình luận</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-03</t>
+  </si>
+  <si>
+    <t>Chỉ nhập khoảng trắng vào nội dung</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-04</t>
+  </si>
+  <si>
+    <t>Xác nhận rằng hệ thống hiển thị thông báo lỗi khi khách hàng không nhập họ tên</t>
+  </si>
+  <si>
+    <t>Không nhập họ tên</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-05</t>
+  </si>
+  <si>
+    <t>Xác nhận rằng hệ thống hiển thị thông báo lỗi khi khách hàng chỉ nhập khoảng trắng vào trường họ tên</t>
+  </si>
+  <si>
+    <t>Chỉ nhập khoảng trắng vào trường họ tên</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-06</t>
+  </si>
+  <si>
+    <t>Xác nhận rằng hệ thống hiển thị thông báo lỗi khi khách hàng nhập nội dung có ký tự ít hơn 10</t>
+  </si>
+  <si>
+    <t>Cho hỏi</t>
+  </si>
+  <si>
+    <t>Nhập nội dung bình luận ít hơn 10 ký tự</t>
+  </si>
+  <si>
+    <t>Truy cập</t>
   </si>
   <si>
     <t>https://www.dienmayxanh.com/</t>
   </si>
   <si>
-    <t>Chọn xem danh sách sản phẩm trong danh mục</t>
-  </si>
-  <si>
-    <t>Lọc nước</t>
-  </si>
-  <si>
-    <t>Chọn hãng</t>
-  </si>
-  <si>
-    <t>Kangaroo</t>
-  </si>
-  <si>
-    <t>Nhấn chọn danh sách sản phẩm trong danh mục</t>
-  </si>
-  <si>
-    <t>Hệ thống chỉ hiển thị danh sách những sản phẩm máy lọc nước kangaroo</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị toàn bộ sản phẩm lọc nước hiện có</t>
-  </si>
-  <si>
-    <t>Xác nhận hệ thống hiển thị danh sách sản phẩm theo giá tiền từ cao đến thấp</t>
-  </si>
-  <si>
-    <t>Xác nhận hệ thống hiển thị danh sách sản phẩm theo giá tiền từ thấp đến cao</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị toàn bộ sản phẩm lọc nước hiện có với sắp xếp theo giá tiền từ thấp đến cao</t>
-  </si>
-  <si>
-    <t>Chọn xếp theo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chọn sắp xếp </t>
-  </si>
-  <si>
-    <t>Giá thấp đến cao</t>
-  </si>
-  <si>
-    <t>Giá cao đến thấp</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị toàn bộ sản phẩm lọc nước hiện có với sắp xếp theo giá tiền từ cao đến thấp</t>
-  </si>
-  <si>
-    <t>Số lượng hiển thị phải đúng với số lượng tổng sản phẩm</t>
-  </si>
-  <si>
-    <t>Xác nhận số lượng trên breadcrumb và ở trước filter bằng với số lượng sản phẩm mà hệ thống hiển thị</t>
-  </si>
-  <si>
-    <t>Hệ thống hiển thị breadcrumb và ở trước filter có số lượng bằng số lượng sản phẩm đang hiển thị</t>
+    <t>Change test data, expected result</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Cảm ơn quý khách đã để lại bình luận, bình luận sẽ được kiểm duyệt và cập nhật lên web.</t>
+  </si>
+  <si>
+    <t>Vui lòng nhập nội dung</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo ở text box nhập bình luận</t>
+  </si>
+  <si>
+    <t>Hiển thị alert thông báo</t>
+  </si>
+  <si>
+    <t>Vui lòng nhập họ tên.</t>
+  </si>
+  <si>
+    <t>Nội dung bình luận quá ngắn</t>
+  </si>
+  <si>
+    <t>Test Cases for 'Comment' function</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -299,7 +350,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +534,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -525,7 +582,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1030,6 +1087,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1040,6 +1108,30 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1052,7 +1144,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1145,12 +1237,18 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1163,197 +1261,230 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1381,6 +1512,104 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57032</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFD06778-00A9-4D7D-8192-2FECEE4591FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="11639432" cy="6082144"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12740</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>31172</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E80A6C29-F87E-412D-AC03-27D16938FCE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="923"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7063740"/>
+          <a:ext cx="11595140" cy="6134792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1649,15 +1878,15 @@
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="53.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="14.44140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="30.33203125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="53.5546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="21" x14ac:dyDescent="0.3">
@@ -1669,12 +1898,12 @@
       <c r="E1" s="51"/>
     </row>
     <row r="2" spans="2:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
@@ -1709,20 +1938,28 @@
         <v>7</v>
       </c>
       <c r="C6" s="7">
-        <v>44150</v>
+        <v>44140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="7">
+        <v>44178</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
@@ -1743,12 +1980,12 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
+      <c r="B11" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
     </row>
     <row r="12" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
@@ -1757,12 +1994,12 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58"/>
+      <c r="B13" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="61"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
@@ -1771,54 +2008,54 @@
       <c r="C14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="48"/>
+      <c r="D14" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="63"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="65"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="65"/>
     </row>
     <row r="19" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1835,137 +2072,134 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F3" sqref="F3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="8.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="16.109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="28.44140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="38.6640625" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="13.109375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="13.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="A1" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="69" t="s">
+      <c r="A2" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="77"/>
       <c r="E2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
+        <v>16</v>
+      </c>
+      <c r="F2" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="76"/>
+      <c r="A3" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="81"/>
+      <c r="C3" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="83"/>
       <c r="E3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78"/>
+        <v>18</v>
+      </c>
+      <c r="F3" s="82"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:9" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62">
-        <v>44150</v>
-      </c>
-      <c r="D4" s="63"/>
+      <c r="A4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69">
+        <v>44140</v>
+      </c>
+      <c r="D4" s="70"/>
       <c r="E4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="65"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="F4" s="69"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
     </row>
     <row r="7" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
+      <c r="A7" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
     </row>
     <row r="8" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1973,21 +2207,21 @@
         <v>1</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="23" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="20"/>
     </row>
@@ -1996,17 +2230,17 @@
         <v>2</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="23" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20">
@@ -2019,23 +2253,46 @@
         <v>3</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="23" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20">
+        <v>2</v>
+      </c>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20">
         <v>1</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I12" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2053,18 +2310,19 @@
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E11" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E12" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"LooknFeel, Positive, Negative, Boundary"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F11" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F12" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"High, Medium, Low"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B9" location="'Test Case'!B4" display="TR-DMX-VLP-01" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B10:B11" location="'Test Case'!B4" display="TR-Fancy-SO-01" xr:uid="{38F6A6A4-1B99-4A1B-AA63-231A554C849F}"/>
-    <hyperlink ref="B10" location="'Test Case'!B9" display="TR-DMX-VLP-02" xr:uid="{5E2DC872-05E6-4080-BE3C-3A683E752B64}"/>
-    <hyperlink ref="B11" location="'Test Case'!B15" display="TR-DMX-VLP-03" xr:uid="{C08E5C9B-AAA4-4BA1-B32A-E2B26A5FF0FD}"/>
+    <hyperlink ref="B9" location="'Test Case'!B4" display="TR-Fancy-SO-01" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B10:B11" location="'Test Case'!B4" display="TR-Fancy-SO-01" xr:uid="{D8EAF582-19E6-4CB1-85C5-94B30BB4D612}"/>
+    <hyperlink ref="B12" location="'Test Case'!B39" display="TR-DMX-BL-04" xr:uid="{3FE78DBE-7BE2-4328-9A58-94ACFF41661C}"/>
+    <hyperlink ref="B11" location="'Test Case'!B25" display="TR-DMX-BL-03" xr:uid="{3F501244-95B6-4A64-AD2F-91734832F201}"/>
+    <hyperlink ref="B10" location="'Test Case'!B11" display="TR-DMX-BL-02" xr:uid="{77E943FC-3CED-4D9E-8178-18FBB6332266}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2072,388 +2330,936 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="8.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="27" width="31.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="36.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.88671875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="21.33203125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="23.21875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="15.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="8.33203125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="27" width="31.33203125" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="19.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="22.0" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="27" width="27.33203125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="102" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="106" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="107"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+    </row>
+    <row r="4" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="103">
+        <v>1</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="93" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86">
-        <v>1</v>
-      </c>
-      <c r="B4" s="79" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="88" t="s">
+      <c r="E4" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="85"/>
       <c r="F4" s="31">
         <v>1</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="86"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="85"/>
+      <c r="G4" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="45"/>
+      <c r="J4" s="39"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="103"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="28">
         <v>2</v>
       </c>
       <c r="G5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="103"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="28">
+        <v>3</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="46"/>
+      <c r="J6" s="36"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="103"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="28">
+        <v>4</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="46"/>
+      <c r="J7" s="36"/>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="103"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="28">
+        <v>5</v>
+      </c>
+      <c r="G8" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H8" s="30"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="36"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="103"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="28">
+        <v>6</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="47"/>
+      <c r="J9" s="36"/>
+    </row>
+    <row r="10" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="103"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="28">
+        <v>7</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="103">
+        <v>2</v>
+      </c>
+      <c r="B11" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="103"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="28">
+        <v>2</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="103"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="28">
+        <v>3</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="103"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="28">
+        <v>4</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="46"/>
+      <c r="J14" s="36"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="103"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="28">
+        <v>5</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="36"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="103"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="28">
+        <v>6</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="47"/>
+      <c r="J16" s="36"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="112"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="41">
+        <v>7</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="86">
+        <v>3</v>
+      </c>
+      <c r="B18" s="109"/>
+      <c r="C18" s="93" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="31">
+        <v>1</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="32"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="39"/>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="87"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="28">
+        <v>2</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="87"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="28">
+        <v>3</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="87"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="28">
+        <v>4</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="46"/>
+      <c r="J21" s="36"/>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="87"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="28">
+        <v>5</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="36"/>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="87"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="28">
+        <v>6</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="47"/>
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="88"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="41">
+        <v>7</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="43"/>
+      <c r="I24" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="98">
+        <v>4</v>
+      </c>
+      <c r="B25" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="31">
+        <v>1</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="32"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="39"/>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="99"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="28">
+        <v>2</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="99"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="28">
+        <v>3</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I27" s="46"/>
+      <c r="J27" s="36"/>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="99"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="28">
+        <v>4</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="30"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="36"/>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="99"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="28">
+        <v>5</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="30"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="36"/>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="99"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="28">
+        <v>6</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="40" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="82">
+      <c r="I30" s="47"/>
+      <c r="J30" s="36"/>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="98"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="28">
+        <v>7</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="33"/>
+      <c r="I31" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="J31" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="86">
+        <v>5</v>
+      </c>
+      <c r="B32" s="96"/>
+      <c r="C32" s="93" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="31">
+        <v>1</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="32"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="39"/>
+    </row>
+    <row r="33" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="87"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="92"/>
+      <c r="F33" s="28">
         <v>2</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="88" t="s">
+      <c r="G33" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="1" customFormat="1" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="87"/>
+      <c r="B34" s="96"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="28">
+        <v>3</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I34" s="46"/>
+      <c r="J34" s="36"/>
+    </row>
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="87"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="28">
+        <v>4</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="30"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="36"/>
+    </row>
+    <row r="36" spans="1:10" s="1" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="87"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="28">
+        <v>5</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="30"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="36"/>
+    </row>
+    <row r="37" spans="1:10" s="1" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="87"/>
+      <c r="B37" s="96"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="28">
+        <v>6</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="47"/>
+      <c r="J37" s="36"/>
+    </row>
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="88"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="91"/>
+      <c r="E38" s="92"/>
+      <c r="F38" s="28">
+        <v>7</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="33"/>
+      <c r="I38" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="1" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="86">
+        <v>6</v>
+      </c>
+      <c r="B39" s="95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="31">
+        <v>1</v>
+      </c>
+      <c r="G39" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="85"/>
-      <c r="F6" s="31">
-        <v>1</v>
-      </c>
-      <c r="G6" s="33" t="s">
+      <c r="H39" s="32"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="39"/>
+    </row>
+    <row r="40" spans="1:10" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="87"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="28">
+        <v>2</v>
+      </c>
+      <c r="G40" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H40" s="30"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="37"/>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="83"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="28">
-        <v>2</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="34"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="84"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="38">
+    </row>
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="87"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="28">
         <v>3</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G41" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I41" s="46"/>
+      <c r="J41" s="36"/>
+    </row>
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="87"/>
+      <c r="B42" s="96"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="28">
+        <v>4</v>
+      </c>
+      <c r="G42" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H42" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I42" s="46"/>
+      <c r="J42" s="36"/>
+    </row>
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="87"/>
+      <c r="B43" s="96"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="28">
+        <v>5</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" s="30"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="36"/>
+    </row>
+    <row r="44" spans="1:10" s="1" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="87"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="94"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="28">
+        <v>6</v>
+      </c>
+      <c r="G44" s="29" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="100">
-        <v>3</v>
-      </c>
-      <c r="B9" s="97" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="87" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="88" t="s">
+      <c r="H44" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" s="47"/>
+      <c r="J44" s="36"/>
+    </row>
+    <row r="45" spans="1:10" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="88"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="113">
+        <v>7</v>
+      </c>
+      <c r="G45" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="31">
-        <v>1</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="37"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="101"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="28">
-        <v>2</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="34"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="100"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="28">
-        <v>3</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="82">
-        <v>4</v>
-      </c>
-      <c r="B12" s="98"/>
-      <c r="C12" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="94" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="85"/>
-      <c r="F12" s="31">
-        <v>1</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="37"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="83"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="28">
-        <v>2</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="84"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="28">
-        <v>3</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="82">
-        <v>5</v>
-      </c>
-      <c r="B15" s="97" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="87" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="94" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="85"/>
-      <c r="F15" s="31">
-        <v>1</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="37"/>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="84"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="42">
-        <v>2</v>
-      </c>
-      <c r="G16" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>74</v>
+      <c r="H45" s="33"/>
+      <c r="I45" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="J45" s="38" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+  <mergeCells count="31">
+    <mergeCell ref="B11:B24"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="E11:E17"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="C11:C17"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="E4:E10"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="D39:D45"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="E39:E45"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B25:B38"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{DB457306-E916-4A45-9B9A-A836984F0BD6}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{58E0D713-8D85-4071-B4E2-8034046C7733}"/>
-    <hyperlink ref="H12" r:id="rId3" xr:uid="{CC93244B-4F6D-4B1E-9F8F-0010B4168B21}"/>
-    <hyperlink ref="H9" r:id="rId4" xr:uid="{E94D457F-C729-41FF-BFA5-A671E6059E6C}"/>
-    <hyperlink ref="H15" r:id="rId5" xr:uid="{0EE36D6F-D509-428D-8B0A-494A1F14B541}"/>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{F250E7E1-3187-4C99-893C-AB1ACFCF73F3}"/>
+    <hyperlink ref="H16" r:id="rId2" xr:uid="{A4988E84-36F8-4EA1-9087-B3B649E81796}"/>
+    <hyperlink ref="H30" r:id="rId3" xr:uid="{F5D32A15-CB07-412C-BFDA-F4A2701E31E3}"/>
+    <hyperlink ref="H23" r:id="rId4" xr:uid="{CEB97D7D-5718-404D-838B-B1E1D7BBDFE8}"/>
+    <hyperlink ref="H37" r:id="rId5" xr:uid="{815853EB-8AFB-45A7-A607-B870C17A549A}"/>
+    <hyperlink ref="H44" r:id="rId6" xr:uid="{42073164-4C67-420B-A18F-2590F44553C0}"/>
+    <hyperlink ref="H4" r:id="rId7" xr:uid="{5AF52FF2-CA19-4513-AAE8-451FE3F2DE0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f7c1022657b138b79f35a4326fa0dc9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c089ff6982c627c0778789fcc62b4c69" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -2611,15 +3417,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2627,6 +3424,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06066F44-28EF-4989-9E2D-F3C30A4D0D5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BCDA75-5053-4A00-AC56-8B4371FB5F69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2644,14 +3449,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06066F44-28EF-4989-9E2D-F3C30A4D0D5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6459A90D-25B3-4765-A81F-CB2B8DBDBF37}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
modify column according to changes of file test excution & add write link image when test fail
</commit_message>
<xml_diff>
--- a/DienmayXANH-FunctionalTestExecution.xlsx
+++ b/DienmayXANH-FunctionalTestExecution.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A1FACB-3F5B-4B4C-BF1D-14CEF675D067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FFED71-C915-4758-B984-6A752B82259D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
   <si>
     <t>Test type: Functiontal test case</t>
   </si>
@@ -228,24 +228,300 @@
     <t>#</t>
   </si>
   <si>
+    <t>Function</t>
+  </si>
+  <si>
     <t>TCs</t>
   </si>
   <si>
-    <t xml:space="preserve">Complexity </t>
-  </si>
-  <si>
     <t>Responsible tester</t>
   </si>
   <si>
+    <t>Test case name</t>
+  </si>
+  <si>
     <t>Test case ID</t>
   </si>
   <si>
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
+    <t>Image test case fail</t>
+  </si>
+  <si>
+    <t>Chọn nơi nhận hàng</t>
+  </si>
+  <si>
+    <t>Yen Dang</t>
+  </si>
+  <si>
+    <t>testMainSFWithFullInfor</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-01</t>
+  </si>
+  <si>
+    <t>testSuccessWithOnlyProvince</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-02</t>
+  </si>
+  <si>
+    <t>testSuccessWithoutFillTextboxAddress</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-03</t>
+  </si>
+  <si>
+    <t>testFailWithoutChooseWard</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-04</t>
+  </si>
+  <si>
+    <t>testSuccessUpdateWithOnlyProvinceSubmitBefor</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-05</t>
+  </si>
+  <si>
+    <t>testSuccessUpdateByClickOnButonChange</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-06</t>
+  </si>
+  <si>
+    <t>testSuccessUpdateByClickOnDropBoxProvince</t>
+  </si>
+  <si>
+    <t>TC-DMX-CNNH-07</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Lan Phuong</t>
+  </si>
+  <si>
+    <t>testLoggedinSuccessfully</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-01</t>
+  </si>
+  <si>
+    <t>testPhoneNumbersWithLetters</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-02</t>
+  </si>
+  <si>
+    <t>testPhoneNumberWithSpecialCharacters</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-03</t>
+  </si>
+  <si>
+    <t>testWrongPhoneNumber</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-04</t>
+  </si>
+  <si>
+    <t>testDoNotEnterPhoneNumber</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-05</t>
+  </si>
+  <si>
+    <t>testEnterSpace</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-06</t>
+  </si>
+  <si>
+    <t>testWrongOTP</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-07</t>
+  </si>
+  <si>
+    <t>testDoNotEnterEnoughOTP</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-08</t>
+  </si>
+  <si>
+    <t>testOTPHasLetters</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-09</t>
+  </si>
+  <si>
+    <t>testOTPHasSpecialCharacters</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-10</t>
+  </si>
+  <si>
+    <t>testOTPEntersSpace</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-11</t>
+  </si>
+  <si>
+    <t>testDoNotEnterOTP</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-12</t>
+  </si>
+  <si>
+    <t>testNoticeOfResendingOTP</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-13</t>
+  </si>
+  <si>
+    <t>testEnterKey</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-14</t>
+  </si>
+  <si>
+    <t>testTitle</t>
+  </si>
+  <si>
+    <t>TR-DMX-Login-15</t>
+  </si>
+  <si>
+    <t>Liên hệ, góp ý</t>
+  </si>
+  <si>
+    <t>Thanh Nhan</t>
+  </si>
+  <si>
+    <t>Bình luận</t>
+  </si>
+  <si>
+    <t>Nhi Phan</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-01</t>
+  </si>
+  <si>
+    <t>testWithoutCommentContent</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-02</t>
+  </si>
+  <si>
+    <t>testOnlySpaceCommentContent</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-03</t>
+  </si>
+  <si>
+    <t>testWithoutName</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-04</t>
+  </si>
+  <si>
+    <t>testOnlySpaceName</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-05</t>
+  </si>
+  <si>
+    <t>testContentCommentIsLessThan10Characters</t>
+  </si>
+  <si>
+    <t>TC-DMX-BL-06</t>
+  </si>
+  <si>
+    <t>Xem danh sách sản phẩm theo hãng</t>
+  </si>
+  <si>
+    <t>Nhi Phan, Thanh Nhan</t>
+  </si>
+  <si>
+    <t>testShowAllProduct</t>
+  </si>
+  <si>
+    <t>TC-DMX-VLP-01</t>
+  </si>
+  <si>
+    <t>testShowAllProductOfBrand</t>
+  </si>
+  <si>
+    <t>TC-DMX-VLP-02</t>
+  </si>
+  <si>
+    <t>testViewWithSortPriceDescending</t>
+  </si>
+  <si>
+    <t>TC-DMX-VLP-03</t>
+  </si>
+  <si>
+    <t>testViewWithSortPriceAscending</t>
+  </si>
+  <si>
+    <t>TC-DMX-VLP-04</t>
+  </si>
+  <si>
+    <t>testQuantity</t>
+  </si>
+  <si>
+    <t>TC-DMX-VLP-05</t>
+  </si>
+  <si>
+    <t>Xem sản phẩm qua danh sách sản phẩm</t>
+  </si>
+  <si>
+    <t>testSuccessViewProductByList</t>
+  </si>
+  <si>
+    <t>TC-DMX-VPBLP-01</t>
+  </si>
+  <si>
+    <t>Mở liên kết</t>
+  </si>
+  <si>
+    <t>testLinkFacebook</t>
+  </si>
+  <si>
+    <t>TC-DMX-Link-01</t>
+  </si>
+  <si>
+    <t>testLinkYoutube</t>
+  </si>
+  <si>
+    <t>TC-DMX-Link-02</t>
+  </si>
+  <si>
+    <t>testLinkMaiAm</t>
+  </si>
+  <si>
+    <t>TC-DMX-Link-03</t>
+  </si>
+  <si>
+    <t>testLinkTgdd</t>
+  </si>
+  <si>
+    <t>TC-DMX-Link-04</t>
+  </si>
+  <si>
+    <t>testLinkBachHoaXanh</t>
+  </si>
+  <si>
+    <t>TC-DMX-Link-05</t>
+  </si>
+  <si>
     <t>Defect ID</t>
   </si>
   <si>
@@ -279,139 +555,56 @@
     <t>Date closed</t>
   </si>
   <si>
-    <t>Chọn nơi nhận hàng</t>
-  </si>
-  <si>
-    <t>Đăng nhập</t>
-  </si>
-  <si>
-    <t>Liên hệ, góp ý</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Bình luận</t>
-  </si>
-  <si>
-    <t>Xem danh sách sản phẩm theo hãng</t>
-  </si>
-  <si>
-    <t>Xem sản phẩm qua danh sách sản phẩm</t>
-  </si>
-  <si>
-    <t>Mở liên kết</t>
-  </si>
-  <si>
-    <t>Yen Dang</t>
-  </si>
-  <si>
-    <t>Lan Phuong</t>
-  </si>
-  <si>
-    <t>Nhi Phan</t>
-  </si>
-  <si>
-    <t>Thanh Nhan</t>
-  </si>
-  <si>
-    <t>Nhi Phan, Thanh Nhan</t>
-  </si>
-  <si>
-    <t>Test case name</t>
-  </si>
-  <si>
-    <t>TC-DMX-BL-01</t>
-  </si>
-  <si>
-    <t>TC-DMX-BL-02</t>
-  </si>
-  <si>
-    <t>TC-DMX-BL-03</t>
-  </si>
-  <si>
-    <t>TC-DMX-BL-04</t>
-  </si>
-  <si>
-    <t>TC-DMX-BL-05</t>
-  </si>
-  <si>
-    <t>TC-DMX-BL-06</t>
-  </si>
-  <si>
-    <t>testWithoutCommentContent</t>
-  </si>
-  <si>
-    <t>testOnlySpaceCommentContent</t>
-  </si>
-  <si>
-    <t>testWithoutName</t>
-  </si>
-  <si>
-    <t>testOnlySpaceName</t>
-  </si>
-  <si>
-    <t>testContentCommentIsLessThan10Characters</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-01</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-02</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-03</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-04</t>
-  </si>
-  <si>
-    <t>TC-DMX-VLP-05</t>
-  </si>
-  <si>
-    <t>testShowAllProduct</t>
-  </si>
-  <si>
-    <t>testShowAllProductOfBrand</t>
-  </si>
-  <si>
-    <t>testViewWithSortPriceDescending</t>
-  </si>
-  <si>
-    <t>testViewWithSortPriceAscending</t>
-  </si>
-  <si>
-    <t>testQuantity</t>
-  </si>
-  <si>
-    <t>Image test case fail</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-01</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-02</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-03</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-04</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-05</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-06</t>
-  </si>
-  <si>
-    <t>TC-DMX-CNNH-07</t>
-  </si>
-  <si>
-    <t>TC-DMX-VPBLP-01</t>
+    <t xml:space="preserve">Máy lọc nước RO hydrogen ion kiềm Kangaroo KG100EO 7 lõi
+</t>
+  </si>
+  <si>
+    <t>496 Dương Quảng Hàm, Phường 6, Quận Gò Vấp, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Đồng Nai</t>
+  </si>
+  <si>
+    <t>Phường 15, Quận Bình Thạnh, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Vui lòng chọn phường xã</t>
+  </si>
+  <si>
+    <t>Xã Tân Đức, Huyện Hàm Tân, Bình Thuận</t>
+  </si>
+  <si>
+    <t>17 Đội Mũ, Phường Đội Cấn, Quận Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>Bắc Kạn</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị breadcrumb và ở trước filter có số lượng bằng số lượng sản phẩm đang hiển thị</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị toàn bộ sản phẩm lọc nước hiện có với sắp xếp theo giá tiền từ thấp đến cao</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị toàn bộ sản phẩm lọc nước hiện có với sắp xếp theo giá tiền từ cao đến thấp</t>
+  </si>
+  <si>
+    <t>Vui lòng nhập nội dung</t>
+  </si>
+  <si>
+    <t>Vui lòng nhập họ tên.</t>
+  </si>
+  <si>
+    <t>Nội dung bình luận quá ngắn</t>
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>DienMayXanh\screenshots\TC-DMX-VLP-05-testQuantity.png</t>
   </si>
 </sst>
 </file>
@@ -421,7 +614,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +690,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF70AD47"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF70AD47"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -536,7 +758,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1013,13 +1235,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1053,9 +1379,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1078,9 +1401,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1306,18 +1626,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1339,9 +1653,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1354,9 +1665,106 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1364,43 +1772,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3097,7 +3484,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5237,112 +5624,112 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="3.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="2.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="3.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="2.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="8.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-    </row>
-    <row r="2" spans="2:12" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="C2" s="50" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="2:12" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="C2" s="48" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="96"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="22"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="96"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="13" t="s">
         <v>7</v>
       </c>
@@ -5354,36 +5741,36 @@
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="47"/>
+      <c r="L11" s="45"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="37" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="46" t="s">
+      <c r="K12" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="48"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="37" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="12"/>
@@ -5391,226 +5778,226 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="22"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="46" t="s">
+      <c r="K13" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="47"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="46" t="s">
+      <c r="K14" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="47"/>
+      <c r="L14" s="45"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="37" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="46" t="s">
+      <c r="K15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="25"/>
+      <c r="L15" s="24"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="37" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="37" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="22"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
     </row>
     <row r="35" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="13"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
-      <c r="F36" s="22"/>
+      <c r="F36" s="21"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="11"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="22"/>
+      <c r="F37" s="21"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
-      <c r="F39" s="22"/>
+      <c r="F39" s="21"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
-      <c r="C40" s="39"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="22"/>
+      <c r="F40" s="21"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
-      <c r="C41" s="39"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
-      <c r="F41" s="22"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
-      <c r="C42" s="39"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="22"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="95"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="93"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5633,911 +6020,1040 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I42" sqref="I42:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="20" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="5.44140625" style="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.44140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.109375" style="21" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.109375" style="37" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.5546875" style="37" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.6640625" style="32" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="19" width="3.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="17" width="5.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="30" width="12.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="20" width="42.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="30" width="17.44140625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="35" width="32.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="30" width="14.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="65.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="146">
+        <v>1</v>
+      </c>
+      <c r="B2" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="149">
+        <v>7</v>
+      </c>
+      <c r="D2" s="152" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="142" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="33"/>
+      <c r="H2" s="139" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="147"/>
+      <c r="B3" s="155"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="143" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="118" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="97"/>
+      <c r="H3" s="140" t="s">
+        <v>132</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="J3" s="113"/>
+    </row>
+    <row r="4" spans="1:12" s="21" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="147"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="153"/>
+      <c r="E4" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="97"/>
+      <c r="H4" s="140" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="29"/>
+      <c r="J4" s="113"/>
+    </row>
+    <row r="5" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="147"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="118" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="97"/>
+      <c r="H5" s="138" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="29"/>
+      <c r="J5" s="113"/>
+    </row>
+    <row r="6" spans="1:12" s="21" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="147"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="140" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" s="29"/>
+      <c r="J6" s="113"/>
+    </row>
+    <row r="7" spans="1:12" s="21" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="147"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="143" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="130" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="140" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="J7" s="109"/>
+    </row>
+    <row r="8" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="148"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="154"/>
+      <c r="E8" s="144" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="131" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="141" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="27"/>
+      <c r="J8" s="111"/>
+    </row>
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="146">
+        <v>2</v>
+      </c>
+      <c r="B9" s="155" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="149">
+        <v>15</v>
+      </c>
+      <c r="D9" s="152" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="126"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="147"/>
+      <c r="B10" s="155"/>
+      <c r="C10" s="150"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="124" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="28" t="s">
+      <c r="G10" s="127"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="99"/>
+    </row>
+    <row r="11" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="147"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="124" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="133" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="127"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="99"/>
+    </row>
+    <row r="12" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="147"/>
+      <c r="B12" s="155"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="124" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="133" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="127"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="99"/>
+    </row>
+    <row r="13" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="147"/>
+      <c r="B13" s="155"/>
+      <c r="C13" s="150"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="133" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="127"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="99"/>
+    </row>
+    <row r="14" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="147"/>
+      <c r="B14" s="155"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="124" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="133" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="127"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="99"/>
+    </row>
+    <row r="15" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="147"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="124" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="127"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="99"/>
+    </row>
+    <row r="16" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="147"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="150"/>
+      <c r="D16" s="153"/>
+      <c r="E16" s="124" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="133" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="127"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="99"/>
+    </row>
+    <row r="17" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="147"/>
+      <c r="B17" s="155"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="124" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="133" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="127"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="99"/>
+    </row>
+    <row r="18" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="147"/>
+      <c r="B18" s="155"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="153"/>
+      <c r="E18" s="124" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="133" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="127"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="99"/>
+    </row>
+    <row r="19" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="147"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="153"/>
+      <c r="E19" s="124" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="133" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="127"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="99"/>
+    </row>
+    <row r="20" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="147"/>
+      <c r="B20" s="155"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="124" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="133" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="128"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="99"/>
+    </row>
+    <row r="21" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="147"/>
+      <c r="B21" s="155"/>
+      <c r="C21" s="150"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="124" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="133" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-    </row>
-    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128">
+      <c r="G21" s="127"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="99"/>
+    </row>
+    <row r="22" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="147"/>
+      <c r="B22" s="155"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="153"/>
+      <c r="E22" s="124" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="127"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="99"/>
+    </row>
+    <row r="23" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="148"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="151"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="125" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="135" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="129"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="100"/>
+    </row>
+    <row r="24" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="158">
+        <v>3</v>
+      </c>
+      <c r="B24" s="157" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="149">
+        <v>10</v>
+      </c>
+      <c r="D24" s="152" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="106"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="107"/>
+    </row>
+    <row r="25" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="159"/>
+      <c r="B25" s="155"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="109"/>
+    </row>
+    <row r="26" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="159"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="150"/>
+      <c r="D26" s="153"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="109"/>
+    </row>
+    <row r="27" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="159"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="150"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="109"/>
+    </row>
+    <row r="28" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="159"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="109"/>
+    </row>
+    <row r="29" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="159"/>
+      <c r="B29" s="155"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="109"/>
+    </row>
+    <row r="30" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="159"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="109"/>
+    </row>
+    <row r="31" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="159"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="153"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="109"/>
+    </row>
+    <row r="32" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="159"/>
+      <c r="B32" s="155"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="153"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="109"/>
+    </row>
+    <row r="33" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="160"/>
+      <c r="B33" s="156"/>
+      <c r="C33" s="151"/>
+      <c r="D33" s="154"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="119"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="111"/>
+    </row>
+    <row r="34" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="158">
+        <v>4</v>
+      </c>
+      <c r="B34" s="157" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="149">
+        <v>6</v>
+      </c>
+      <c r="D34" s="152" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="106"/>
+      <c r="F34" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="107"/>
+    </row>
+    <row r="35" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="159"/>
+      <c r="B35" s="155"/>
+      <c r="C35" s="150"/>
+      <c r="D35" s="153"/>
+      <c r="E35" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="118" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" s="109"/>
+    </row>
+    <row r="36" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="159"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="150"/>
+      <c r="D36" s="153"/>
+      <c r="E36" s="108" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="118" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="I36" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J36" s="109"/>
+    </row>
+    <row r="37" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="159"/>
+      <c r="B37" s="155"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="153"/>
+      <c r="E37" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="118" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="H37" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I37" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37" s="109"/>
+    </row>
+    <row r="38" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="159"/>
+      <c r="B38" s="155"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="153"/>
+      <c r="E38" s="108" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="118" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="109"/>
+    </row>
+    <row r="39" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="160"/>
+      <c r="B39" s="156"/>
+      <c r="C39" s="151"/>
+      <c r="D39" s="154"/>
+      <c r="E39" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="119" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="J39" s="111"/>
+    </row>
+    <row r="40" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="158">
+        <v>5</v>
+      </c>
+      <c r="B40" s="157" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="149">
+        <v>5</v>
+      </c>
+      <c r="D40" s="152" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="107"/>
+    </row>
+    <row r="41" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="159"/>
+      <c r="B41" s="155"/>
+      <c r="C41" s="150"/>
+      <c r="D41" s="153"/>
+      <c r="E41" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="118" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="109"/>
+    </row>
+    <row r="42" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="159"/>
+      <c r="B42" s="155"/>
+      <c r="C42" s="150"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="118" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J42" s="109"/>
+    </row>
+    <row r="43" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="159"/>
+      <c r="B43" s="155"/>
+      <c r="C43" s="150"/>
+      <c r="D43" s="153"/>
+      <c r="E43" s="108" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="118" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="H43" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J43" s="109"/>
+    </row>
+    <row r="44" spans="1:10" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="160"/>
+      <c r="B44" s="156"/>
+      <c r="C44" s="151"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="110" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="119" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="J44" s="111" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="21" customFormat="1" ht="39.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="101">
+        <v>6</v>
+      </c>
+      <c r="B45" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="103">
         <v>1</v>
       </c>
-      <c r="B2" s="137" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="127">
+      <c r="D45" s="112" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="122" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" s="121" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="104"/>
+      <c r="H45" s="137" t="s">
+        <v>130</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="J45" s="105"/>
+    </row>
+    <row r="46" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="159">
         <v>7</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="110"/>
-      <c r="G2" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-    </row>
-    <row r="3" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="129"/>
-      <c r="B3" s="132"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="118"/>
-    </row>
-    <row r="4" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="129"/>
-      <c r="B4" s="132"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="99"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="118"/>
-    </row>
-    <row r="5" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="129"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="118"/>
-    </row>
-    <row r="6" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="129"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="99"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="118"/>
-    </row>
-    <row r="7" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="113"/>
-    </row>
-    <row r="8" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="130"/>
-      <c r="B8" s="133"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="115"/>
-    </row>
-    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="128">
-        <v>2</v>
-      </c>
-      <c r="B9" s="132" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="127">
-        <v>15</v>
-      </c>
-      <c r="D9" s="127"/>
-      <c r="E9" s="131" t="s">
+      <c r="B46" s="155" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="150">
+        <v>5</v>
+      </c>
+      <c r="D46" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="110"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="97"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="129"/>
-      <c r="B10" s="132"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="101"/>
-    </row>
-    <row r="11" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="129"/>
-      <c r="B11" s="132"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="101"/>
-    </row>
-    <row r="12" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="129"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="101"/>
-    </row>
-    <row r="13" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="129"/>
-      <c r="B13" s="132"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="101"/>
-    </row>
-    <row r="14" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="129"/>
-      <c r="B14" s="132"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="101"/>
-    </row>
-    <row r="15" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="129"/>
-      <c r="B15" s="132"/>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="101"/>
-    </row>
-    <row r="16" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="129"/>
-      <c r="B16" s="132"/>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="101"/>
-    </row>
-    <row r="17" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="129"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="125"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="101"/>
-    </row>
-    <row r="18" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="129"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="101"/>
-    </row>
-    <row r="19" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="129"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="101"/>
-    </row>
-    <row r="20" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="129"/>
-      <c r="B20" s="132"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="101"/>
-    </row>
-    <row r="21" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="129"/>
-      <c r="B21" s="132"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="101"/>
-    </row>
-    <row r="22" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="129"/>
-      <c r="B22" s="132"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="112"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="101"/>
-    </row>
-    <row r="23" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="130"/>
-      <c r="B23" s="133"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="114"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="102"/>
-    </row>
-    <row r="24" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="136">
-        <v>3</v>
-      </c>
-      <c r="B24" s="137" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="127">
-        <v>10</v>
-      </c>
-      <c r="D24" s="127"/>
-      <c r="E24" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="110"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="111"/>
-    </row>
-    <row r="25" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="134"/>
-      <c r="B25" s="132"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="125"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="113"/>
-    </row>
-    <row r="26" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="134"/>
-      <c r="B26" s="132"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="113"/>
-    </row>
-    <row r="27" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="134"/>
-      <c r="B27" s="132"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="113"/>
-    </row>
-    <row r="28" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="134"/>
-      <c r="B28" s="132"/>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="113"/>
-    </row>
-    <row r="29" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="134"/>
-      <c r="B29" s="132"/>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="113"/>
-    </row>
-    <row r="30" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="134"/>
-      <c r="B30" s="132"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="113"/>
-    </row>
-    <row r="31" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="134"/>
-      <c r="B31" s="132"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="112"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="113"/>
-    </row>
-    <row r="32" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="134"/>
-      <c r="B32" s="132"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="113"/>
-    </row>
-    <row r="33" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="135"/>
-      <c r="B33" s="133"/>
-      <c r="C33" s="126"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="114"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="115"/>
-    </row>
-    <row r="34" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="136">
-        <v>4</v>
-      </c>
-      <c r="B34" s="137" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="127">
-        <v>6</v>
-      </c>
-      <c r="D34" s="127"/>
-      <c r="E34" s="131" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="110"/>
-      <c r="G34" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="H34" s="35"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="111"/>
-    </row>
-    <row r="35" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="134"/>
-      <c r="B35" s="132"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="112" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="H35" s="36"/>
-      <c r="I35" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35" s="113"/>
-    </row>
-    <row r="36" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="134"/>
-      <c r="B36" s="132"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="112" t="s">
-        <v>59</v>
-      </c>
-      <c r="G36" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H36" s="36"/>
-      <c r="I36" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J36" s="113"/>
-    </row>
-    <row r="37" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="134"/>
-      <c r="B37" s="132"/>
-      <c r="C37" s="125"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="112" t="s">
-        <v>60</v>
-      </c>
-      <c r="G37" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="H37" s="36"/>
-      <c r="I37" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J37" s="113"/>
-    </row>
-    <row r="38" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="134"/>
-      <c r="B38" s="132"/>
-      <c r="C38" s="125"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="123"/>
-      <c r="F38" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="G38" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="H38" s="36"/>
-      <c r="I38" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J38" s="113"/>
-    </row>
-    <row r="39" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="135"/>
-      <c r="B39" s="133"/>
-      <c r="C39" s="126"/>
-      <c r="D39" s="126"/>
-      <c r="E39" s="124"/>
-      <c r="F39" s="114" t="s">
-        <v>62</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="34"/>
-      <c r="I39" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" s="115"/>
-    </row>
-    <row r="40" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="136">
-        <v>5</v>
-      </c>
-      <c r="B40" s="137" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="127">
-        <v>5</v>
-      </c>
-      <c r="D40" s="127"/>
-      <c r="E40" s="131" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="110" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H40" s="35"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="111"/>
-    </row>
-    <row r="41" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="134"/>
-      <c r="B41" s="132"/>
-      <c r="C41" s="125"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="H41" s="36"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="113"/>
-    </row>
-    <row r="42" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="134"/>
-      <c r="B42" s="132"/>
-      <c r="C42" s="125"/>
-      <c r="D42" s="125"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="112" t="s">
-        <v>70</v>
-      </c>
-      <c r="G42" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="H42" s="36"/>
-      <c r="I42" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J42" s="113"/>
-    </row>
-    <row r="43" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="134"/>
-      <c r="B43" s="132"/>
-      <c r="C43" s="125"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="123"/>
-      <c r="F43" s="112" t="s">
-        <v>71</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="36"/>
-      <c r="I43" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J43" s="113"/>
-    </row>
-    <row r="44" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="135"/>
-      <c r="B44" s="133"/>
-      <c r="C44" s="126"/>
-      <c r="D44" s="126"/>
-      <c r="E44" s="124"/>
-      <c r="F44" s="114" t="s">
-        <v>72</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H44" s="34"/>
-      <c r="I44" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J44" s="115"/>
-    </row>
-    <row r="45" spans="1:10" s="22" customFormat="1" ht="39.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="103">
-        <v>6</v>
-      </c>
-      <c r="B45" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="105">
-        <v>1</v>
-      </c>
-      <c r="D45" s="105"/>
-      <c r="E45" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" s="105"/>
-      <c r="G45" s="106" t="s">
-        <v>81</v>
-      </c>
-      <c r="H45" s="107"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="108"/>
-    </row>
-    <row r="46" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="134">
-        <v>7</v>
-      </c>
-      <c r="B46" s="132" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="125">
-        <v>5</v>
-      </c>
-      <c r="D46" s="125"/>
-      <c r="E46" s="123" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="44"/>
-      <c r="G46" s="109"/>
-      <c r="H46" s="119"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="111"/>
-    </row>
-    <row r="47" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="134"/>
-      <c r="B47" s="132"/>
-      <c r="C47" s="125"/>
-      <c r="D47" s="125"/>
-      <c r="E47" s="123"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="120"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="113"/>
-    </row>
-    <row r="48" spans="1:10" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="134"/>
-      <c r="B48" s="132"/>
-      <c r="C48" s="125"/>
-      <c r="D48" s="125"/>
-      <c r="E48" s="123"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="120"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="113"/>
-    </row>
-    <row r="49" spans="1:12" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="134"/>
-      <c r="B49" s="132"/>
-      <c r="C49" s="125"/>
-      <c r="D49" s="125"/>
-      <c r="E49" s="123"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="120"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="113"/>
-    </row>
-    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="135"/>
-      <c r="B50" s="133"/>
-      <c r="C50" s="126"/>
-      <c r="D50" s="126"/>
-      <c r="E50" s="124"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="121"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="115"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
+      <c r="E46" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="114"/>
+      <c r="H46" s="114"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="107"/>
+    </row>
+    <row r="47" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="159"/>
+      <c r="B47" s="155"/>
+      <c r="C47" s="150"/>
+      <c r="D47" s="153"/>
+      <c r="E47" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="109"/>
+    </row>
+    <row r="48" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="159"/>
+      <c r="B48" s="155"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="153"/>
+      <c r="E48" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="115"/>
+      <c r="H48" s="115"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="109"/>
+    </row>
+    <row r="49" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="159"/>
+      <c r="B49" s="155"/>
+      <c r="C49" s="150"/>
+      <c r="D49" s="153"/>
+      <c r="E49" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="136" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" s="115"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="109"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="160"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="151"/>
+      <c r="D50" s="154"/>
+      <c r="E50" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="131" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="116"/>
+      <c r="H50" s="116"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="111"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="51"/>
-      <c r="B51" s="22"/>
-      <c r="D51" s="21"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="52"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="21"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="51"/>
-      <c r="B52" s="22"/>
-      <c r="D52" s="21"/>
-      <c r="F52" s="19" t="s">
+      <c r="A52" s="49"/>
+      <c r="B52" s="21"/>
+      <c r="E52" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
-    </row>
-    <row r="53" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="51"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="32"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+    </row>
+    <row r="53" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="49"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="30"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="51"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="32"/>
+    <row r="54" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="49"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="30"/>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="51"/>
-      <c r="B55" s="22"/>
-      <c r="D55" s="21"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="51"/>
-      <c r="B56" s="22"/>
-      <c r="D56" s="21"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="22"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="51"/>
-      <c r="B57" s="22"/>
-      <c r="D57" s="21"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="22"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="51"/>
-      <c r="B58" s="22"/>
-      <c r="D58" s="21"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="51"/>
-      <c r="B59" s="22"/>
-      <c r="D59" s="21"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="51"/>
-      <c r="B60" s="22"/>
-      <c r="D60" s="21"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
+      <c r="A60" s="49"/>
+      <c r="B60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="51"/>
-      <c r="B61" s="22"/>
-      <c r="D61" s="21"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="22"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="51"/>
-      <c r="B62" s="22"/>
-      <c r="D62" s="21"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
+      <c r="A62" s="49"/>
+      <c r="B62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="24">
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="A9:A23"/>
+    <mergeCell ref="D9:D23"/>
+    <mergeCell ref="C9:C23"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="D24:D33"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="D40:D44"/>
     <mergeCell ref="B9:B23"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C24:C33"/>
     <mergeCell ref="B24:B33"/>
-    <mergeCell ref="A24:A33"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="D40:D44"/>
-    <mergeCell ref="D24:D33"/>
-    <mergeCell ref="E24:E33"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="E40:E44"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="C46:C50"/>
     <mergeCell ref="D2:D8"/>
-    <mergeCell ref="A9:A23"/>
-    <mergeCell ref="E9:E23"/>
-    <mergeCell ref="C9:C23"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="D9:D23"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="B40:B44"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="I2:I50">
@@ -6578,275 +7094,275 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="58" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.88671875" style="83" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.109375" style="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.88671875" style="58" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.88671875" style="85" collapsed="1"/>
-    <col min="8" max="8" width="13.109375" style="86" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.6640625" style="86" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5546875" style="86" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.88671875" style="87" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.88671875" style="58" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="8.88671875" style="58" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="56" width="9.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="81" width="38.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="56" width="43.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="56" width="25.88671875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="82" width="11.109375" collapsed="true"/>
+    <col min="7" max="7" style="83" width="8.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="84" width="13.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="84" width="11.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="84" width="13.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="85" width="12.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="56" width="10.88671875" collapsed="true"/>
+    <col min="13" max="16384" style="56" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
+      <c r="A1" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="62"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="66"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="62"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="64"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="62"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="64"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="62"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="64"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="64"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="62"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="64"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="62"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="64"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="62"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="64"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="62"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="64"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="64"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="66"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="62"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="66"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="74"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
-    </row>
-    <row r="17" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="79"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="64"/>
-    </row>
-    <row r="18" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="93"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="62"/>
+    </row>
+    <row r="17" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="77"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+    </row>
+    <row r="18" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="86"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="91"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -6947,9 +7463,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7117,26 +7636,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5589AC8F-1D80-4A3C-B04F-4E3B731AFF63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4D3485E-123B-42CD-A17B-4E9A5EAAA4CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7160,9 +7668,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4D3485E-123B-42CD-A17B-4E9A5EAAA4CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5589AC8F-1D80-4A3C-B04F-4E3B731AFF63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
apply data driven testing for ViewProductThroughList class
</commit_message>
<xml_diff>
--- a/DienmayXANH-FunctionalTestExecution.xlsx
+++ b/DienmayXANH-FunctionalTestExecution.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185DFB24-0C47-4320-B7D9-FFEA06B0446B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDA511D-2245-4BCB-9D49-A481B0ABDDE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
   <si>
     <t>Test type: Functiontal test case</t>
   </si>
@@ -547,25 +547,19 @@
     <t>17 Đội Mũ, Phường Đội Cấn, Quận Ba Đình, Hà Nội</t>
   </si>
   <si>
-    <t>Máy lọc nước RO hydrogen ion kiềm Kangaroo KG100EO 7 lõi</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>Bình Thuận</t>
+    <t>Hệ thống hiển thị đúng thông tin chi tiết sản phẩm đó</t>
+  </si>
+  <si>
+    <t>TP. Hồ Chí Minh</t>
   </si>
   <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>DienMayXanh\screenshots\screenshot-testSuccessUpdateWithOnlyProvinceSubmitBefor.png</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>DienMayXanh\screenshots\screenshot-testSuccessUpdateByClickOnButonChange.png</t>
+    <t>DienMayXanh\screenshots\screenshot-testSuccessWithoutFillTextboxAddress.png</t>
   </si>
 </sst>
 </file>
@@ -1698,6 +1692,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1705,42 +1735,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5974,8 +5968,8 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G8"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6026,7 +6020,7 @@
       <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="157">
+      <c r="A2" s="145">
         <v>1</v>
       </c>
       <c r="B2" s="156" t="s">
@@ -6051,14 +6045,14 @@
         <v>125</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" s="107"/>
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="158"/>
+      <c r="A3" s="146"/>
       <c r="B3" s="154"/>
       <c r="C3" s="149"/>
       <c r="D3" s="152"/>
@@ -6075,12 +6069,12 @@
         <v>122</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J3" s="113"/>
     </row>
     <row r="4" spans="1:12" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="158"/>
+      <c r="A4" s="146"/>
       <c r="B4" s="154"/>
       <c r="C4" s="149"/>
       <c r="D4" s="152"/>
@@ -6091,18 +6085,20 @@
         <v>37</v>
       </c>
       <c r="G4" s="97" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H4" s="140" t="s">
         <v>120</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="J4" s="113"/>
+        <v>130</v>
+      </c>
+      <c r="J4" s="113" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="5" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="158"/>
+      <c r="A5" s="146"/>
       <c r="B5" s="154"/>
       <c r="C5" s="149"/>
       <c r="D5" s="152"/>
@@ -6119,12 +6115,12 @@
         <v>123</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:12" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="158"/>
+      <c r="A6" s="146"/>
       <c r="B6" s="154"/>
       <c r="C6" s="149"/>
       <c r="D6" s="152"/>
@@ -6141,14 +6137,12 @@
         <v>124</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="113" t="s">
-        <v>131</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="J6" s="113"/>
     </row>
     <row r="7" spans="1:12" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="158"/>
+      <c r="A7" s="146"/>
       <c r="B7" s="154"/>
       <c r="C7" s="149"/>
       <c r="D7" s="152"/>
@@ -6165,14 +6159,12 @@
         <v>126</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="J7" s="109" t="s">
-        <v>133</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="J7" s="109"/>
     </row>
     <row r="8" spans="1:12" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="159"/>
+      <c r="A8" s="147"/>
       <c r="B8" s="155"/>
       <c r="C8" s="150"/>
       <c r="D8" s="153"/>
@@ -6189,12 +6181,12 @@
         <v>121</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8" s="111"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="157">
+      <c r="A9" s="145">
         <v>2</v>
       </c>
       <c r="B9" s="154" t="s">
@@ -6220,7 +6212,7 @@
       <c r="L9" s="21"/>
     </row>
     <row r="10" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="158"/>
+      <c r="A10" s="146"/>
       <c r="B10" s="154"/>
       <c r="C10" s="149"/>
       <c r="D10" s="152"/>
@@ -6236,7 +6228,7 @@
       <c r="J10" s="99"/>
     </row>
     <row r="11" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="158"/>
+      <c r="A11" s="146"/>
       <c r="B11" s="154"/>
       <c r="C11" s="149"/>
       <c r="D11" s="152"/>
@@ -6252,7 +6244,7 @@
       <c r="J11" s="99"/>
     </row>
     <row r="12" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="158"/>
+      <c r="A12" s="146"/>
       <c r="B12" s="154"/>
       <c r="C12" s="149"/>
       <c r="D12" s="152"/>
@@ -6268,7 +6260,7 @@
       <c r="J12" s="99"/>
     </row>
     <row r="13" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="158"/>
+      <c r="A13" s="146"/>
       <c r="B13" s="154"/>
       <c r="C13" s="149"/>
       <c r="D13" s="152"/>
@@ -6284,7 +6276,7 @@
       <c r="J13" s="99"/>
     </row>
     <row r="14" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="158"/>
+      <c r="A14" s="146"/>
       <c r="B14" s="154"/>
       <c r="C14" s="149"/>
       <c r="D14" s="152"/>
@@ -6300,7 +6292,7 @@
       <c r="J14" s="99"/>
     </row>
     <row r="15" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="158"/>
+      <c r="A15" s="146"/>
       <c r="B15" s="154"/>
       <c r="C15" s="149"/>
       <c r="D15" s="152"/>
@@ -6316,7 +6308,7 @@
       <c r="J15" s="99"/>
     </row>
     <row r="16" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="158"/>
+      <c r="A16" s="146"/>
       <c r="B16" s="154"/>
       <c r="C16" s="149"/>
       <c r="D16" s="152"/>
@@ -6332,7 +6324,7 @@
       <c r="J16" s="99"/>
     </row>
     <row r="17" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="158"/>
+      <c r="A17" s="146"/>
       <c r="B17" s="154"/>
       <c r="C17" s="149"/>
       <c r="D17" s="152"/>
@@ -6348,7 +6340,7 @@
       <c r="J17" s="99"/>
     </row>
     <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="158"/>
+      <c r="A18" s="146"/>
       <c r="B18" s="154"/>
       <c r="C18" s="149"/>
       <c r="D18" s="152"/>
@@ -6364,7 +6356,7 @@
       <c r="J18" s="99"/>
     </row>
     <row r="19" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="158"/>
+      <c r="A19" s="146"/>
       <c r="B19" s="154"/>
       <c r="C19" s="149"/>
       <c r="D19" s="152"/>
@@ -6380,7 +6372,7 @@
       <c r="J19" s="99"/>
     </row>
     <row r="20" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="158"/>
+      <c r="A20" s="146"/>
       <c r="B20" s="154"/>
       <c r="C20" s="149"/>
       <c r="D20" s="152"/>
@@ -6396,7 +6388,7 @@
       <c r="J20" s="99"/>
     </row>
     <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="158"/>
+      <c r="A21" s="146"/>
       <c r="B21" s="154"/>
       <c r="C21" s="149"/>
       <c r="D21" s="152"/>
@@ -6412,7 +6404,7 @@
       <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="158"/>
+      <c r="A22" s="146"/>
       <c r="B22" s="154"/>
       <c r="C22" s="149"/>
       <c r="D22" s="152"/>
@@ -6428,7 +6420,7 @@
       <c r="J22" s="99"/>
     </row>
     <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="159"/>
+      <c r="A23" s="147"/>
       <c r="B23" s="155"/>
       <c r="C23" s="150"/>
       <c r="D23" s="153"/>
@@ -6444,7 +6436,7 @@
       <c r="J23" s="100"/>
     </row>
     <row r="24" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="145">
+      <c r="A24" s="157">
         <v>3</v>
       </c>
       <c r="B24" s="156" t="s">
@@ -6464,7 +6456,7 @@
       <c r="J24" s="107"/>
     </row>
     <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="146"/>
+      <c r="A25" s="158"/>
       <c r="B25" s="154"/>
       <c r="C25" s="149"/>
       <c r="D25" s="152"/>
@@ -6476,7 +6468,7 @@
       <c r="J25" s="109"/>
     </row>
     <row r="26" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="146"/>
+      <c r="A26" s="158"/>
       <c r="B26" s="154"/>
       <c r="C26" s="149"/>
       <c r="D26" s="152"/>
@@ -6488,7 +6480,7 @@
       <c r="J26" s="109"/>
     </row>
     <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="146"/>
+      <c r="A27" s="158"/>
       <c r="B27" s="154"/>
       <c r="C27" s="149"/>
       <c r="D27" s="152"/>
@@ -6500,7 +6492,7 @@
       <c r="J27" s="109"/>
     </row>
     <row r="28" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="146"/>
+      <c r="A28" s="158"/>
       <c r="B28" s="154"/>
       <c r="C28" s="149"/>
       <c r="D28" s="152"/>
@@ -6512,7 +6504,7 @@
       <c r="J28" s="109"/>
     </row>
     <row r="29" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="146"/>
+      <c r="A29" s="158"/>
       <c r="B29" s="154"/>
       <c r="C29" s="149"/>
       <c r="D29" s="152"/>
@@ -6524,7 +6516,7 @@
       <c r="J29" s="109"/>
     </row>
     <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="146"/>
+      <c r="A30" s="158"/>
       <c r="B30" s="154"/>
       <c r="C30" s="149"/>
       <c r="D30" s="152"/>
@@ -6536,7 +6528,7 @@
       <c r="J30" s="109"/>
     </row>
     <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="146"/>
+      <c r="A31" s="158"/>
       <c r="B31" s="154"/>
       <c r="C31" s="149"/>
       <c r="D31" s="152"/>
@@ -6548,7 +6540,7 @@
       <c r="J31" s="109"/>
     </row>
     <row r="32" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="146"/>
+      <c r="A32" s="158"/>
       <c r="B32" s="154"/>
       <c r="C32" s="149"/>
       <c r="D32" s="152"/>
@@ -6560,7 +6552,7 @@
       <c r="J32" s="109"/>
     </row>
     <row r="33" spans="1:10" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="147"/>
+      <c r="A33" s="159"/>
       <c r="B33" s="155"/>
       <c r="C33" s="150"/>
       <c r="D33" s="153"/>
@@ -6572,7 +6564,7 @@
       <c r="J33" s="111"/>
     </row>
     <row r="34" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="145">
+      <c r="A34" s="157">
         <v>4</v>
       </c>
       <c r="B34" s="156" t="s">
@@ -6594,7 +6586,7 @@
       <c r="J34" s="107"/>
     </row>
     <row r="35" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="146"/>
+      <c r="A35" s="158"/>
       <c r="B35" s="154"/>
       <c r="C35" s="149"/>
       <c r="D35" s="152"/>
@@ -6610,7 +6602,7 @@
       <c r="J35" s="109"/>
     </row>
     <row r="36" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="146"/>
+      <c r="A36" s="158"/>
       <c r="B36" s="154"/>
       <c r="C36" s="149"/>
       <c r="D36" s="152"/>
@@ -6626,7 +6618,7 @@
       <c r="J36" s="109"/>
     </row>
     <row r="37" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="146"/>
+      <c r="A37" s="158"/>
       <c r="B37" s="154"/>
       <c r="C37" s="149"/>
       <c r="D37" s="152"/>
@@ -6642,7 +6634,7 @@
       <c r="J37" s="109"/>
     </row>
     <row r="38" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="146"/>
+      <c r="A38" s="158"/>
       <c r="B38" s="154"/>
       <c r="C38" s="149"/>
       <c r="D38" s="152"/>
@@ -6658,7 +6650,7 @@
       <c r="J38" s="109"/>
     </row>
     <row r="39" spans="1:10" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="147"/>
+      <c r="A39" s="159"/>
       <c r="B39" s="155"/>
       <c r="C39" s="150"/>
       <c r="D39" s="153"/>
@@ -6674,7 +6666,7 @@
       <c r="J39" s="111"/>
     </row>
     <row r="40" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="145">
+      <c r="A40" s="157">
         <v>5</v>
       </c>
       <c r="B40" s="156" t="s">
@@ -6698,7 +6690,7 @@
       <c r="J40" s="107"/>
     </row>
     <row r="41" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="146"/>
+      <c r="A41" s="158"/>
       <c r="B41" s="154"/>
       <c r="C41" s="149"/>
       <c r="D41" s="152"/>
@@ -6714,7 +6706,7 @@
       <c r="J41" s="109"/>
     </row>
     <row r="42" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="146"/>
+      <c r="A42" s="158"/>
       <c r="B42" s="154"/>
       <c r="C42" s="149"/>
       <c r="D42" s="152"/>
@@ -6730,7 +6722,7 @@
       <c r="J42" s="109"/>
     </row>
     <row r="43" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="146"/>
+      <c r="A43" s="158"/>
       <c r="B43" s="154"/>
       <c r="C43" s="149"/>
       <c r="D43" s="152"/>
@@ -6746,7 +6738,7 @@
       <c r="J43" s="109"/>
     </row>
     <row r="44" spans="1:10" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="147"/>
+      <c r="A44" s="159"/>
       <c r="B44" s="155"/>
       <c r="C44" s="150"/>
       <c r="D44" s="153"/>
@@ -6780,15 +6772,19 @@
       <c r="F45" s="121" t="s">
         <v>107</v>
       </c>
-      <c r="G45" s="104"/>
+      <c r="G45" s="104" t="s">
+        <v>128</v>
+      </c>
       <c r="H45" s="143" t="s">
+        <v>128</v>
+      </c>
+      <c r="I45" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="I45" s="28"/>
       <c r="J45" s="105"/>
     </row>
     <row r="46" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="146">
+      <c r="A46" s="158">
         <v>7</v>
       </c>
       <c r="B46" s="154" t="s">
@@ -6808,7 +6804,7 @@
       <c r="J46" s="107"/>
     </row>
     <row r="47" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="146"/>
+      <c r="A47" s="158"/>
       <c r="B47" s="154"/>
       <c r="C47" s="149"/>
       <c r="D47" s="152"/>
@@ -6820,7 +6816,7 @@
       <c r="J47" s="109"/>
     </row>
     <row r="48" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="146"/>
+      <c r="A48" s="158"/>
       <c r="B48" s="154"/>
       <c r="C48" s="149"/>
       <c r="D48" s="152"/>
@@ -6832,7 +6828,7 @@
       <c r="J48" s="109"/>
     </row>
     <row r="49" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="146"/>
+      <c r="A49" s="158"/>
       <c r="B49" s="154"/>
       <c r="C49" s="149"/>
       <c r="D49" s="152"/>
@@ -6844,7 +6840,7 @@
       <c r="J49" s="109"/>
     </row>
     <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="147"/>
+      <c r="A50" s="159"/>
       <c r="B50" s="155"/>
       <c r="C50" s="150"/>
       <c r="D50" s="153"/>
@@ -6961,6 +6957,7 @@
     <mergeCell ref="C40:C44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A24:A33"/>
+    <mergeCell ref="A2:A8"/>
     <mergeCell ref="C2:C8"/>
     <mergeCell ref="D34:D39"/>
     <mergeCell ref="D40:D44"/>
@@ -6969,7 +6966,6 @@
     <mergeCell ref="C24:C33"/>
     <mergeCell ref="B24:B33"/>
     <mergeCell ref="D2:D8"/>
-    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="I2:I50">

</xml_diff>

<commit_message>
remove setExcel in @BeforeClass
</commit_message>
<xml_diff>
--- a/DienmayXANH-FunctionalTestExecution.xlsx
+++ b/DienmayXANH-FunctionalTestExecution.xlsx
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="147">
   <si>
     <t>Test type: Functiontal test case</t>
   </si>
@@ -6647,7 +6647,7 @@
         <v>141</v>
       </c>
       <c r="I36" s="29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J36" s="109"/>
     </row>
@@ -6669,7 +6669,7 @@
         <v>142</v>
       </c>
       <c r="I37" s="29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J37" s="109"/>
     </row>
@@ -6691,7 +6691,7 @@
         <v>142</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J38" s="109"/>
     </row>
@@ -6713,7 +6713,7 @@
         <v>143</v>
       </c>
       <c r="I39" s="27" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J39" s="111"/>
     </row>
@@ -6797,7 +6797,7 @@
         <v>139</v>
       </c>
       <c r="I43" s="29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J43" s="109"/>
     </row>

</xml_diff>

<commit_message>
done done data driven
</commit_message>
<xml_diff>
--- a/DienmayXANH-FunctionalTestExecution.xlsx
+++ b/DienmayXANH-FunctionalTestExecution.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
     <sheet name="Detailed status" sheetId="5" r:id="rId2"/>
     <sheet name="Bug report" sheetId="7" r:id="rId3"/>
+    <sheet name="danh so thu tu" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Author">"$#REF!.$#REF!$#REF!"</definedName>
@@ -31,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -244,8 +244,35 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng test case</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="165">
   <si>
     <t>Test type: Functiontal test case</t>
   </si>
@@ -457,7 +484,7 @@
     <t>TR-DMX-Login-07</t>
   </si>
   <si>
-    <t>Mã xác nhận không đúng, vui lòng thử lại</t>
+    <t>* Mã xác nhận không đúng, vui lòng thử lại.</t>
   </si>
   <si>
     <t>testDoNotEnterEnoughOTP</t>
@@ -466,7 +493,7 @@
     <t>TR-DMX-Login-08</t>
   </si>
   <si>
-    <t>Vui lòng nhập mã OTP</t>
+    <t>* Vui lòng nhập mã OTP.</t>
   </si>
   <si>
     <t>testOTPHasLetters</t>
@@ -514,6 +541,9 @@
     <t>TR-DMX-Login-15</t>
   </si>
   <si>
+    <t>Lịch sử mua hàng | Dienmayxanh.com | Dienmayxanh.com</t>
+  </si>
+  <si>
     <t>Liên hệ, góp ý</t>
   </si>
   <si>
@@ -622,8 +652,7 @@
     <t>TC-DMX-VPBLP-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Máy lọc nước RO hydrogen ion kiềm Kangaroo KG100EO 7 lõi
-</t>
+    <t>Hệ thống hiển thị đúng thông tin chi tiết sản phẩm đó</t>
   </si>
   <si>
     <t>Mở liên kết</t>
@@ -692,7 +721,52 @@
     <t>Date closed</t>
   </si>
   <si>
-    <t>Lịch sử mua hàng | Dienmayxanh.com | Dienmayxanh.com</t>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>01_01</t>
+  </si>
+  <si>
+    <t>01_02</t>
+  </si>
+  <si>
+    <t>01_03</t>
+  </si>
+  <si>
+    <t>01_04</t>
+  </si>
+  <si>
+    <t>01_05</t>
+  </si>
+  <si>
+    <t>01_06</t>
+  </si>
+  <si>
+    <t>01_07</t>
+  </si>
+  <si>
+    <t>Hệ thống mở tab Facebook Điện máy xanh.</t>
+  </si>
+  <si>
+    <t>Hệ thống mở tab YouTube Điện máy xanh.</t>
+  </si>
+  <si>
+    <t>Hệ thống mở tab MÁI ẤM Thế Giới Di Động.</t>
+  </si>
+  <si>
+    <t>Hệ thống mở tab thegioididong.com.</t>
+  </si>
+  <si>
+    <t>Hệ thống mở tab Bách hóa XANH.</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
@@ -782,6 +856,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -801,11 +876,13 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF70AD47"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -853,7 +930,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1460,13 +1537,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1881,6 +1989,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1937,7 +2072,40 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="84">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5363,26 +5531,30 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B10:H17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B10:H17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="83" tableBorderDxfId="82">
   <tableColumns count="7">
-    <tableColumn id="1" name="Column1" headerRowDxfId="77" dataDxfId="76"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="75" dataDxfId="74"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="73" dataDxfId="72"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="71" dataDxfId="70"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="69"/>
-    <tableColumn id="6" name="Column6" headerRowDxfId="68"/>
-    <tableColumn id="7" name="Column7" headerRowDxfId="67"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="81" dataDxfId="80"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="79" dataDxfId="78"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="77" dataDxfId="76"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="75" dataDxfId="74"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="73"/>
+    <tableColumn id="6" name="Column6" headerRowDxfId="72"/>
+    <tableColumn id="7" name="Column7" headerRowDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="J10:L15" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="J10:L15" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="70">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="65"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="64" dataDxfId="63"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="69"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="68" dataDxfId="67"/>
     <tableColumn id="3" name="Column3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5390,7 +5562,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C4:D7" totalsRowShown="0" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C4:D7" totalsRowShown="0" tableBorderDxfId="66">
   <tableColumns count="2">
     <tableColumn id="1" name="Overall progress of the QA cycle(Ontime, delayed, Stopped)"/>
     <tableColumn id="2" name="On time"/>
@@ -5400,30 +5572,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table33" displayName="Table33" ref="B35:D42" headerRowCount="0" totalsRowShown="0" headerRowDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table33" displayName="Table33" ref="B35:D42" headerRowCount="0" totalsRowShown="0" headerRowDxfId="65" tableBorderDxfId="64">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="59" dataDxfId="58"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="57" dataDxfId="56"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="59" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K18" totalsRowCount="1" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K18" totalsRowCount="1" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="Defect ID" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" name="Defect Description" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" name="Steps to reproduce" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="9" name="Reference" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" name="Severity" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="10" name="Priority" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="State" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" name="Detected by" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="11" name="Assigned to" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="8" name="Date open" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Date closed" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Defect ID" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Defect Description" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Steps to reproduce" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="9" name="Reference" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" name="Severity" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="10" name="Priority" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" name="State" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="6" name="Detected by" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="11" name="Assigned to" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="8" name="Date open" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" name="Date closed" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5770,6 +5942,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2020-05-12T04:48:20.37" personId="{00000000-0000-0000-0000-000000000000}" id="{7D4A09FA-348F-4DFD-BDBF-157CDBF33C71}">
+    <text>Số lượng test case</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L53"/>
@@ -5780,15 +5960,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="3.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="2.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="41.33203125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="9.5546875" collapsed="false"/>
+    <col min="7" max="8" customWidth="true" width="9.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="3.6640625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="2.109375" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="26.88671875" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="8.33203125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
@@ -5823,8 +6003,8 @@
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="150"/>
+      <c r="G4" s="159"/>
+      <c r="H4" s="159"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
@@ -6176,21 +6356,21 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46:I50"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="19" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="5.44140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" style="30" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="42.109375" style="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.44140625" style="30" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="32.5546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.88671875" style="30" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="19" width="3.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="14.44140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="17" width="5.44140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="30" width="12.5546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="20" width="42.109375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="30" width="17.44140625" collapsed="false"/>
+    <col min="7" max="8" customWidth="true" style="35" width="32.5546875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="30" width="14.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="65.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6228,16 +6408,16 @@
       <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="151">
+      <c r="A2" s="160">
         <v>1</v>
       </c>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="154">
+      <c r="C2" s="163">
         <v>7</v>
       </c>
-      <c r="D2" s="157" t="s">
+      <c r="D2" s="166" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="136" t="s">
@@ -6256,10 +6436,10 @@
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="152"/>
-      <c r="B3" s="160"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="158"/>
+      <c r="A3" s="161"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="167"/>
       <c r="E3" s="137" t="s">
         <v>35</v>
       </c>
@@ -6274,10 +6454,10 @@
       <c r="J3" s="111"/>
     </row>
     <row r="4" spans="1:12" s="21" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="152"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="158"/>
+      <c r="A4" s="161"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="167"/>
       <c r="E4" s="137" t="s">
         <v>38</v>
       </c>
@@ -6292,10 +6472,10 @@
       <c r="J4" s="111"/>
     </row>
     <row r="5" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="152"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="158"/>
+      <c r="A5" s="161"/>
+      <c r="B5" s="169"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="137" t="s">
         <v>41</v>
       </c>
@@ -6306,14 +6486,16 @@
       <c r="H5" s="132" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="29" t="s">
+        <v>151</v>
+      </c>
       <c r="J5" s="111"/>
     </row>
     <row r="6" spans="1:12" s="21" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="152"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="158"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="137" t="s">
         <v>44</v>
       </c>
@@ -6324,14 +6506,16 @@
       <c r="H6" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="29" t="s">
+        <v>150</v>
+      </c>
       <c r="J6" s="111"/>
     </row>
     <row r="7" spans="1:12" s="21" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="152"/>
-      <c r="B7" s="160"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="158"/>
+      <c r="A7" s="161"/>
+      <c r="B7" s="169"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="167"/>
       <c r="E7" s="137" t="s">
         <v>47</v>
       </c>
@@ -6342,14 +6526,16 @@
       <c r="H7" s="134" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="29" t="s">
+        <v>149</v>
+      </c>
       <c r="J7" s="107"/>
     </row>
     <row r="8" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="153"/>
-      <c r="B8" s="161"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="159"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="138" t="s">
         <v>50</v>
       </c>
@@ -6364,16 +6550,16 @@
       <c r="J8" s="109"/>
     </row>
     <row r="9" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="151">
+      <c r="A9" s="160">
         <v>2</v>
       </c>
-      <c r="B9" s="160" t="s">
+      <c r="B9" s="169" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="154">
+      <c r="C9" s="163">
         <v>15</v>
       </c>
-      <c r="D9" s="157" t="s">
+      <c r="D9" s="166" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="121" t="s">
@@ -6389,10 +6575,10 @@
       <c r="L9" s="21"/>
     </row>
     <row r="10" spans="1:12" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="152"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="155"/>
-      <c r="D10" s="158"/>
+      <c r="A10" s="161"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="167"/>
       <c r="E10" s="122" t="s">
         <v>57</v>
       </c>
@@ -6407,28 +6593,32 @@
       <c r="J10" s="97"/>
     </row>
     <row r="11" spans="1:12" s="21" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="152"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="158"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="169"/>
+      <c r="C11" s="164"/>
+      <c r="D11" s="167"/>
       <c r="E11" s="122" t="s">
         <v>60</v>
       </c>
       <c r="F11" s="140" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="142"/>
+      <c r="G11" s="142" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="143"/>
+      <c r="I11" s="143" t="s">
+        <v>164</v>
+      </c>
       <c r="J11" s="97"/>
     </row>
     <row r="12" spans="1:12" s="21" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="152"/>
-      <c r="B12" s="160"/>
-      <c r="C12" s="155"/>
-      <c r="D12" s="158"/>
+      <c r="A12" s="161"/>
+      <c r="B12" s="169"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="167"/>
       <c r="E12" s="122" t="s">
         <v>62</v>
       </c>
@@ -6443,10 +6633,10 @@
       <c r="J12" s="97"/>
     </row>
     <row r="13" spans="1:12" s="21" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="152"/>
-      <c r="B13" s="160"/>
-      <c r="C13" s="155"/>
-      <c r="D13" s="158"/>
+      <c r="A13" s="161"/>
+      <c r="B13" s="169"/>
+      <c r="C13" s="164"/>
+      <c r="D13" s="167"/>
       <c r="E13" s="122" t="s">
         <v>64</v>
       </c>
@@ -6461,10 +6651,10 @@
       <c r="J13" s="97"/>
     </row>
     <row r="14" spans="1:12" s="21" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="152"/>
-      <c r="B14" s="160"/>
-      <c r="C14" s="155"/>
-      <c r="D14" s="158"/>
+      <c r="A14" s="161"/>
+      <c r="B14" s="169"/>
+      <c r="C14" s="164"/>
+      <c r="D14" s="167"/>
       <c r="E14" s="122" t="s">
         <v>66</v>
       </c>
@@ -6479,10 +6669,10 @@
       <c r="J14" s="97"/>
     </row>
     <row r="15" spans="1:12" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="152"/>
-      <c r="B15" s="160"/>
-      <c r="C15" s="155"/>
-      <c r="D15" s="158"/>
+      <c r="A15" s="161"/>
+      <c r="B15" s="169"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="167"/>
       <c r="E15" s="122" t="s">
         <v>68</v>
       </c>
@@ -6497,10 +6687,10 @@
       <c r="J15" s="97"/>
     </row>
     <row r="16" spans="1:12" s="21" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="152"/>
-      <c r="B16" s="160"/>
-      <c r="C16" s="155"/>
-      <c r="D16" s="158"/>
+      <c r="A16" s="161"/>
+      <c r="B16" s="169"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="167"/>
       <c r="E16" s="122" t="s">
         <v>71</v>
       </c>
@@ -6515,10 +6705,10 @@
       <c r="J16" s="97"/>
     </row>
     <row r="17" spans="1:10" s="21" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="152"/>
-      <c r="B17" s="160"/>
-      <c r="C17" s="155"/>
-      <c r="D17" s="158"/>
+      <c r="A17" s="161"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="164"/>
+      <c r="D17" s="167"/>
       <c r="E17" s="122" t="s">
         <v>74</v>
       </c>
@@ -6533,10 +6723,10 @@
       <c r="J17" s="97"/>
     </row>
     <row r="18" spans="1:10" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="152"/>
-      <c r="B18" s="160"/>
-      <c r="C18" s="155"/>
-      <c r="D18" s="158"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="169"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="167"/>
       <c r="E18" s="122" t="s">
         <v>76</v>
       </c>
@@ -6551,10 +6741,10 @@
       <c r="J18" s="97"/>
     </row>
     <row r="19" spans="1:10" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="152"/>
-      <c r="B19" s="160"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="158"/>
+      <c r="A19" s="161"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="164"/>
+      <c r="D19" s="167"/>
       <c r="E19" s="122" t="s">
         <v>78</v>
       </c>
@@ -6569,10 +6759,10 @@
       <c r="J19" s="97"/>
     </row>
     <row r="20" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="152"/>
-      <c r="B20" s="160"/>
-      <c r="C20" s="155"/>
-      <c r="D20" s="158"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="167"/>
       <c r="E20" s="122" t="s">
         <v>80</v>
       </c>
@@ -6587,10 +6777,10 @@
       <c r="J20" s="97"/>
     </row>
     <row r="21" spans="1:10" s="21" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="152"/>
-      <c r="B21" s="160"/>
-      <c r="C21" s="155"/>
-      <c r="D21" s="158"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="167"/>
       <c r="E21" s="122" t="s">
         <v>82</v>
       </c>
@@ -6605,10 +6795,10 @@
       <c r="J21" s="97"/>
     </row>
     <row r="22" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="152"/>
-      <c r="B22" s="160"/>
-      <c r="C22" s="155"/>
-      <c r="D22" s="158"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="164"/>
+      <c r="D22" s="167"/>
       <c r="E22" s="122" t="s">
         <v>85</v>
       </c>
@@ -6621,10 +6811,10 @@
       <c r="J22" s="97"/>
     </row>
     <row r="23" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="153"/>
-      <c r="B23" s="161"/>
-      <c r="C23" s="156"/>
-      <c r="D23" s="159"/>
+      <c r="A23" s="162"/>
+      <c r="B23" s="170"/>
+      <c r="C23" s="165"/>
+      <c r="D23" s="168"/>
       <c r="E23" s="123" t="s">
         <v>87</v>
       </c>
@@ -6633,23 +6823,23 @@
       </c>
       <c r="G23" s="127"/>
       <c r="H23" s="32" t="s">
-        <v>148</v>
+        <v>89</v>
       </c>
       <c r="I23" s="27"/>
       <c r="J23" s="98"/>
     </row>
     <row r="24" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="163">
+      <c r="A24" s="172">
         <v>3</v>
       </c>
-      <c r="B24" s="162" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="154">
+      <c r="B24" s="171" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="163">
         <v>10</v>
       </c>
-      <c r="D24" s="157" t="s">
-        <v>90</v>
+      <c r="D24" s="166" t="s">
+        <v>91</v>
       </c>
       <c r="E24" s="104"/>
       <c r="F24" s="118"/>
@@ -6659,10 +6849,10 @@
       <c r="J24" s="105"/>
     </row>
     <row r="25" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="164"/>
-      <c r="B25" s="160"/>
-      <c r="C25" s="155"/>
-      <c r="D25" s="158"/>
+      <c r="A25" s="173"/>
+      <c r="B25" s="169"/>
+      <c r="C25" s="164"/>
+      <c r="D25" s="167"/>
       <c r="E25" s="106"/>
       <c r="F25" s="116"/>
       <c r="G25" s="34"/>
@@ -6671,10 +6861,10 @@
       <c r="J25" s="107"/>
     </row>
     <row r="26" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="164"/>
-      <c r="B26" s="160"/>
-      <c r="C26" s="155"/>
-      <c r="D26" s="158"/>
+      <c r="A26" s="173"/>
+      <c r="B26" s="169"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="167"/>
       <c r="E26" s="106"/>
       <c r="F26" s="116"/>
       <c r="G26" s="34"/>
@@ -6683,10 +6873,10 @@
       <c r="J26" s="107"/>
     </row>
     <row r="27" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="164"/>
-      <c r="B27" s="160"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="158"/>
+      <c r="A27" s="173"/>
+      <c r="B27" s="169"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="167"/>
       <c r="E27" s="106"/>
       <c r="F27" s="116"/>
       <c r="G27" s="34"/>
@@ -6695,10 +6885,10 @@
       <c r="J27" s="107"/>
     </row>
     <row r="28" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="164"/>
-      <c r="B28" s="160"/>
-      <c r="C28" s="155"/>
-      <c r="D28" s="158"/>
+      <c r="A28" s="173"/>
+      <c r="B28" s="169"/>
+      <c r="C28" s="164"/>
+      <c r="D28" s="167"/>
       <c r="E28" s="106"/>
       <c r="F28" s="116"/>
       <c r="G28" s="34"/>
@@ -6707,10 +6897,10 @@
       <c r="J28" s="107"/>
     </row>
     <row r="29" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="164"/>
-      <c r="B29" s="160"/>
-      <c r="C29" s="155"/>
-      <c r="D29" s="158"/>
+      <c r="A29" s="173"/>
+      <c r="B29" s="169"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="167"/>
       <c r="E29" s="106"/>
       <c r="F29" s="116"/>
       <c r="G29" s="34"/>
@@ -6719,10 +6909,10 @@
       <c r="J29" s="107"/>
     </row>
     <row r="30" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="164"/>
-      <c r="B30" s="160"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="158"/>
+      <c r="A30" s="173"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="167"/>
       <c r="E30" s="106"/>
       <c r="F30" s="116"/>
       <c r="G30" s="34"/>
@@ -6731,10 +6921,10 @@
       <c r="J30" s="107"/>
     </row>
     <row r="31" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="164"/>
-      <c r="B31" s="160"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="158"/>
+      <c r="A31" s="173"/>
+      <c r="B31" s="169"/>
+      <c r="C31" s="164"/>
+      <c r="D31" s="167"/>
       <c r="E31" s="106"/>
       <c r="F31" s="116"/>
       <c r="G31" s="34"/>
@@ -6743,10 +6933,10 @@
       <c r="J31" s="107"/>
     </row>
     <row r="32" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="164"/>
-      <c r="B32" s="160"/>
-      <c r="C32" s="155"/>
-      <c r="D32" s="158"/>
+      <c r="A32" s="173"/>
+      <c r="B32" s="169"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="167"/>
       <c r="E32" s="106"/>
       <c r="F32" s="116"/>
       <c r="G32" s="34"/>
@@ -6755,10 +6945,10 @@
       <c r="J32" s="107"/>
     </row>
     <row r="33" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="165"/>
-      <c r="B33" s="161"/>
-      <c r="C33" s="156"/>
-      <c r="D33" s="159"/>
+      <c r="A33" s="174"/>
+      <c r="B33" s="170"/>
+      <c r="C33" s="165"/>
+      <c r="D33" s="168"/>
       <c r="E33" s="108"/>
       <c r="F33" s="117"/>
       <c r="G33" s="32"/>
@@ -6767,21 +6957,21 @@
       <c r="J33" s="109"/>
     </row>
     <row r="34" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="163">
+      <c r="A34" s="172">
         <v>4</v>
       </c>
-      <c r="B34" s="162" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="154">
+      <c r="B34" s="171" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="163">
         <v>6</v>
       </c>
-      <c r="D34" s="157" t="s">
-        <v>92</v>
+      <c r="D34" s="166" t="s">
+        <v>93</v>
       </c>
       <c r="E34" s="104"/>
       <c r="F34" s="115" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="33"/>
@@ -6789,113 +6979,113 @@
       <c r="J34" s="105"/>
     </row>
     <row r="35" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="164"/>
-      <c r="B35" s="160"/>
-      <c r="C35" s="155"/>
-      <c r="D35" s="158"/>
+      <c r="A35" s="173"/>
+      <c r="B35" s="169"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="167"/>
       <c r="E35" s="106" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F35" s="116" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G35" s="34"/>
       <c r="H35" s="34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I35" s="29"/>
       <c r="J35" s="107"/>
     </row>
     <row r="36" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="164"/>
-      <c r="B36" s="160"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="158"/>
+      <c r="A36" s="173"/>
+      <c r="B36" s="169"/>
+      <c r="C36" s="164"/>
+      <c r="D36" s="167"/>
       <c r="E36" s="106" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F36" s="116" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G36" s="34"/>
       <c r="H36" s="34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I36" s="29"/>
       <c r="J36" s="107"/>
     </row>
     <row r="37" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="164"/>
-      <c r="B37" s="160"/>
-      <c r="C37" s="155"/>
-      <c r="D37" s="158"/>
+      <c r="A37" s="173"/>
+      <c r="B37" s="169"/>
+      <c r="C37" s="164"/>
+      <c r="D37" s="167"/>
       <c r="E37" s="106" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F37" s="116" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G37" s="34"/>
       <c r="H37" s="34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I37" s="29"/>
       <c r="J37" s="107"/>
     </row>
     <row r="38" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="164"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="155"/>
-      <c r="D38" s="158"/>
+      <c r="A38" s="173"/>
+      <c r="B38" s="169"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="167"/>
       <c r="E38" s="106" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F38" s="116" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G38" s="34"/>
       <c r="H38" s="34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I38" s="29"/>
       <c r="J38" s="107"/>
     </row>
     <row r="39" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="165"/>
-      <c r="B39" s="161"/>
-      <c r="C39" s="156"/>
-      <c r="D39" s="159"/>
+      <c r="A39" s="174"/>
+      <c r="B39" s="170"/>
+      <c r="C39" s="165"/>
+      <c r="D39" s="168"/>
       <c r="E39" s="108" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="117" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I39" s="27"/>
       <c r="J39" s="109"/>
     </row>
     <row r="40" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="163">
+      <c r="A40" s="172">
         <v>5</v>
       </c>
-      <c r="B40" s="162" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="154">
+      <c r="B40" s="171" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="163">
         <v>5</v>
       </c>
-      <c r="D40" s="157" t="s">
-        <v>108</v>
+      <c r="D40" s="166" t="s">
+        <v>109</v>
       </c>
       <c r="E40" s="104" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F40" s="115" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G40" s="33"/>
       <c r="H40" s="33"/>
@@ -6903,15 +7093,15 @@
       <c r="J40" s="105"/>
     </row>
     <row r="41" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="164"/>
-      <c r="B41" s="160"/>
-      <c r="C41" s="155"/>
-      <c r="D41" s="158"/>
+      <c r="A41" s="173"/>
+      <c r="B41" s="169"/>
+      <c r="C41" s="164"/>
+      <c r="D41" s="167"/>
       <c r="E41" s="106" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F41" s="116" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
@@ -6919,65 +7109,65 @@
       <c r="J41" s="107"/>
     </row>
     <row r="42" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="164"/>
-      <c r="B42" s="160"/>
-      <c r="C42" s="155"/>
-      <c r="D42" s="158"/>
+      <c r="A42" s="173"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="167"/>
       <c r="E42" s="106" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F42" s="116" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G42" s="34"/>
       <c r="H42" s="34" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I42" s="29"/>
       <c r="J42" s="107"/>
     </row>
     <row r="43" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="164"/>
-      <c r="B43" s="160"/>
-      <c r="C43" s="155"/>
-      <c r="D43" s="158"/>
+      <c r="A43" s="173"/>
+      <c r="B43" s="169"/>
+      <c r="C43" s="164"/>
+      <c r="D43" s="167"/>
       <c r="E43" s="106" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F43" s="116" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I43" s="29"/>
       <c r="J43" s="107"/>
     </row>
     <row r="44" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="165"/>
-      <c r="B44" s="161"/>
-      <c r="C44" s="156"/>
-      <c r="D44" s="159"/>
+      <c r="A44" s="174"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="165"/>
+      <c r="D44" s="168"/>
       <c r="E44" s="108" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F44" s="117" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G44" s="32"/>
       <c r="H44" s="32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I44" s="27"/>
       <c r="J44" s="109"/>
     </row>
-    <row r="45" spans="1:10" s="21" customFormat="1" ht="39.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" s="21" customFormat="1" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="99">
         <v>6</v>
       </c>
       <c r="B45" s="100" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C45" s="101">
         <v>1</v>
@@ -6986,103 +7176,113 @@
         <v>31</v>
       </c>
       <c r="E45" s="120" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F45" s="119" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G45" s="102"/>
       <c r="H45" s="131" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I45" s="28"/>
       <c r="J45" s="103"/>
     </row>
-    <row r="46" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="164">
+    <row r="46" spans="1:10" s="21" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="173">
         <v>7</v>
       </c>
-      <c r="B46" s="160" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="155">
+      <c r="B46" s="169" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="164">
         <v>5</v>
       </c>
-      <c r="D46" s="158" t="s">
+      <c r="D46" s="167" t="s">
         <v>54</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F46" s="115" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G46" s="112"/>
-      <c r="H46" s="112"/>
+      <c r="H46" s="112" t="s">
+        <v>159</v>
+      </c>
       <c r="I46" s="28"/>
       <c r="J46" s="105"/>
     </row>
-    <row r="47" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="164"/>
-      <c r="B47" s="160"/>
-      <c r="C47" s="155"/>
-      <c r="D47" s="158"/>
+    <row r="47" spans="1:10" s="21" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="173"/>
+      <c r="B47" s="169"/>
+      <c r="C47" s="164"/>
+      <c r="D47" s="167"/>
       <c r="E47" s="22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F47" s="116" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G47" s="113"/>
-      <c r="H47" s="113"/>
+      <c r="H47" s="113" t="s">
+        <v>160</v>
+      </c>
       <c r="I47" s="29"/>
       <c r="J47" s="107"/>
     </row>
-    <row r="48" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="164"/>
-      <c r="B48" s="160"/>
-      <c r="C48" s="155"/>
-      <c r="D48" s="158"/>
+    <row r="48" spans="1:10" s="21" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="173"/>
+      <c r="B48" s="169"/>
+      <c r="C48" s="164"/>
+      <c r="D48" s="167"/>
       <c r="E48" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F48" s="116" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G48" s="113"/>
-      <c r="H48" s="113"/>
+      <c r="H48" s="113" t="s">
+        <v>161</v>
+      </c>
       <c r="I48" s="29"/>
       <c r="J48" s="107"/>
     </row>
-    <row r="49" spans="1:12" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="164"/>
-      <c r="B49" s="160"/>
-      <c r="C49" s="155"/>
-      <c r="D49" s="158"/>
+    <row r="49" spans="1:12" s="21" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="173"/>
+      <c r="B49" s="169"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="167"/>
       <c r="E49" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F49" s="116" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G49" s="113"/>
-      <c r="H49" s="113"/>
+      <c r="H49" s="113" t="s">
+        <v>162</v>
+      </c>
       <c r="I49" s="29"/>
       <c r="J49" s="107"/>
     </row>
     <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="165"/>
-      <c r="B50" s="161"/>
-      <c r="C50" s="156"/>
-      <c r="D50" s="159"/>
+      <c r="A50" s="174"/>
+      <c r="B50" s="170"/>
+      <c r="C50" s="165"/>
+      <c r="D50" s="168"/>
       <c r="E50" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F50" s="149" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G50" s="114"/>
-      <c r="H50" s="114"/>
+      <c r="H50" s="114" t="s">
+        <v>163</v>
+      </c>
       <c r="I50" s="27"/>
       <c r="J50" s="109"/>
       <c r="K50" s="21"/>
@@ -7204,18 +7404,18 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="I2:I16 I18:I50">
-    <cfRule type="cellIs" dxfId="53" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="95" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="96" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I16 I18:I50">
-    <cfRule type="cellIs" dxfId="51" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="90" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="92" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7241,53 +7441,53 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="56" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.88671875" style="81" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.109375" style="56" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.88671875" style="56" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.109375" style="82" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.88671875" style="83" collapsed="1"/>
-    <col min="8" max="8" width="13.109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.6640625" style="84" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.88671875" style="85" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.88671875" style="56" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="8.88671875" style="56" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="56" width="9.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="81" width="38.88671875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="56" width="43.109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="56" width="25.88671875" collapsed="false"/>
+    <col min="5" max="6" customWidth="true" style="82" width="11.109375" collapsed="false"/>
+    <col min="7" max="7" style="83" width="8.88671875" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="84" width="13.109375" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="84" width="11.6640625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="84" width="13.5546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="85" width="12.88671875" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="56" width="10.88671875" collapsed="false"/>
+    <col min="13" max="16384" style="56" width="8.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J1" s="54" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K1" s="55" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
@@ -7514,81 +7714,81 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="E2:F17">
-    <cfRule type="cellIs" dxfId="49" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="97" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="98" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="99" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="100" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="101" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="102" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="103" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="104" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="105" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="106" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1 J1:J10 J16:J17 J18:K1048576">
-    <cfRule type="timePeriod" dxfId="39" priority="96" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="43" priority="96" timePeriod="yesterday">
       <formula>FLOOR(J1,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="38" priority="86" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="42" priority="86" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="87" operator="containsText" text="Verified">
+    <cfRule type="containsText" dxfId="41" priority="87" operator="containsText" text="Verified">
       <formula>NOT(ISERROR(SEARCH("Verified",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="88" operator="containsText" text="Reopen">
+    <cfRule type="containsText" dxfId="40" priority="88" operator="containsText" text="Reopen">
       <formula>NOT(ISERROR(SEARCH("Reopen",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="89" operator="containsText" text="Not a bug">
+    <cfRule type="containsText" dxfId="39" priority="89" operator="containsText" text="Not a bug">
       <formula>NOT(ISERROR(SEARCH("Not a bug",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="90" operator="containsText" text="Deferred">
+    <cfRule type="containsText" dxfId="38" priority="90" operator="containsText" text="Deferred">
       <formula>NOT(ISERROR(SEARCH("Deferred",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="91" operator="containsText" text="Duplicate">
+    <cfRule type="containsText" dxfId="37" priority="91" operator="containsText" text="Duplicate">
       <formula>NOT(ISERROR(SEARCH("Duplicate",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="92" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="36" priority="92" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="93" operator="containsText" text="Fixed">
+    <cfRule type="containsText" dxfId="35" priority="93" operator="containsText" text="Fixed">
       <formula>NOT(ISERROR(SEARCH("Fixed",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="94" operator="containsText" text="Assigned">
+    <cfRule type="containsText" dxfId="34" priority="94" operator="containsText" text="Assigned">
       <formula>NOT(ISERROR(SEARCH("Assigned",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="95" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="33" priority="95" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="timePeriod" dxfId="28" priority="75" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="32" priority="75" timePeriod="yesterday">
       <formula>FLOOR(J11,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J15">
-    <cfRule type="timePeriod" dxfId="27" priority="74" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="31" priority="74" timePeriod="yesterday">
       <formula>FLOOR(J12,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7609,16 +7809,1061 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K54"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="49" width="3.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="21" width="14.44140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="17" width="5.44140625" collapsed="false"/>
+    <col min="4" max="5" customWidth="true" style="30" width="12.5546875" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="20" width="42.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="30" width="17.44140625" collapsed="false"/>
+    <col min="8" max="9" customWidth="true" style="35" width="32.5546875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="30" width="14.88671875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="65.0" collapsed="false"/>
+    <col min="12" max="16384" style="21" width="8.88671875" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="160">
+        <v>1</v>
+      </c>
+      <c r="B2" s="171" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="163">
+        <v>7</v>
+      </c>
+      <c r="D2" s="166" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="156" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="136" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="115" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="133" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="28"/>
+      <c r="K2" s="105"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="161"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="157" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="116" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="95"/>
+      <c r="I3" s="134" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="29"/>
+      <c r="K3" s="111"/>
+    </row>
+    <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="161"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="157" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="116" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="95"/>
+      <c r="I4" s="134" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="111"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="161"/>
+      <c r="B5" s="169"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="157" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="137" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="95"/>
+      <c r="I5" s="132" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="K5" s="111"/>
+    </row>
+    <row r="6" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="161"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="157" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="137" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="116" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="95"/>
+      <c r="I6" s="134" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="K6" s="111"/>
+    </row>
+    <row r="7" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="161"/>
+      <c r="B7" s="169"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="157" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="137" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="128" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="134" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="K7" s="107"/>
+    </row>
+    <row r="8" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="162"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="158" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="138" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="129" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="32"/>
+      <c r="I8" s="135" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="109"/>
+    </row>
+    <row r="9" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="160">
+        <v>2</v>
+      </c>
+      <c r="B9" s="169" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="163">
+        <v>15</v>
+      </c>
+      <c r="D9" s="166" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="153"/>
+      <c r="F9" s="121" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="139" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="124"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="96"/>
+    </row>
+    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="161"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="154"/>
+      <c r="F10" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="140" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="142"/>
+      <c r="I10" s="144" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="143"/>
+      <c r="K10" s="97"/>
+    </row>
+    <row r="11" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="161"/>
+      <c r="B11" s="169"/>
+      <c r="C11" s="164"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="122" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="142"/>
+      <c r="I11" s="144" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="143"/>
+      <c r="K11" s="97"/>
+    </row>
+    <row r="12" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="161"/>
+      <c r="B12" s="169"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="140" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="142"/>
+      <c r="I12" s="144" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="143"/>
+      <c r="K12" s="97"/>
+    </row>
+    <row r="13" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="161"/>
+      <c r="B13" s="169"/>
+      <c r="C13" s="164"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="154"/>
+      <c r="F13" s="122" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="140" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="142"/>
+      <c r="I13" s="144" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="143"/>
+      <c r="K13" s="97"/>
+    </row>
+    <row r="14" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="161"/>
+      <c r="B14" s="169"/>
+      <c r="C14" s="164"/>
+      <c r="D14" s="167"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="122" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="140" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="142"/>
+      <c r="I14" s="144" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="143"/>
+      <c r="K14" s="97"/>
+    </row>
+    <row r="15" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="161"/>
+      <c r="B15" s="169"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="122" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="140" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="125"/>
+      <c r="I15" s="145" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="29"/>
+      <c r="K15" s="97"/>
+    </row>
+    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="161"/>
+      <c r="B16" s="169"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="122" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="140" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="125"/>
+      <c r="I16" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="29"/>
+      <c r="K16" s="97"/>
+    </row>
+    <row r="17" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="161"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="164"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="140" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="125"/>
+      <c r="I17" s="146" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="34"/>
+      <c r="K17" s="97"/>
+    </row>
+    <row r="18" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="161"/>
+      <c r="B18" s="169"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="122" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="140" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="125"/>
+      <c r="I18" s="146" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="29"/>
+      <c r="K18" s="97"/>
+    </row>
+    <row r="19" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="161"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="164"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="154"/>
+      <c r="F19" s="122" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="140" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="125"/>
+      <c r="I19" s="146" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="97"/>
+    </row>
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="161"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="167"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="122" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="140" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="126"/>
+      <c r="I20" s="147" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="29"/>
+      <c r="K20" s="97"/>
+    </row>
+    <row r="21" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="161"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="122" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="140" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="142"/>
+      <c r="I21" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="J21" s="143"/>
+      <c r="K21" s="97"/>
+    </row>
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="161"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="164"/>
+      <c r="D22" s="167"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="122" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="125"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="97"/>
+    </row>
+    <row r="23" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="162"/>
+      <c r="B23" s="170"/>
+      <c r="C23" s="165"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="155"/>
+      <c r="F23" s="123" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="130" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="127"/>
+      <c r="I23" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="27"/>
+      <c r="K23" s="98"/>
+    </row>
+    <row r="24" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="172">
+        <v>3</v>
+      </c>
+      <c r="B24" s="171" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="163">
+        <v>10</v>
+      </c>
+      <c r="D24" s="166" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="150"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="105"/>
+    </row>
+    <row r="25" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="173"/>
+      <c r="B25" s="169"/>
+      <c r="C25" s="164"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="107"/>
+    </row>
+    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="173"/>
+      <c r="B26" s="169"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="167"/>
+      <c r="E26" s="151"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="107"/>
+    </row>
+    <row r="27" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="173"/>
+      <c r="B27" s="169"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="107"/>
+    </row>
+    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="173"/>
+      <c r="B28" s="169"/>
+      <c r="C28" s="164"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="151"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="107"/>
+    </row>
+    <row r="29" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="173"/>
+      <c r="B29" s="169"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="107"/>
+    </row>
+    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="173"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="116"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="107"/>
+    </row>
+    <row r="31" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="173"/>
+      <c r="B31" s="169"/>
+      <c r="C31" s="164"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="151"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="107"/>
+    </row>
+    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="173"/>
+      <c r="B32" s="169"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="107"/>
+    </row>
+    <row r="33" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="174"/>
+      <c r="B33" s="170"/>
+      <c r="C33" s="165"/>
+      <c r="D33" s="168"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="117"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="109"/>
+    </row>
+    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="172">
+        <v>4</v>
+      </c>
+      <c r="B34" s="171" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="163">
+        <v>6</v>
+      </c>
+      <c r="D34" s="166" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="150"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="115" t="s">
+        <v>94</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="105"/>
+    </row>
+    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="173"/>
+      <c r="B35" s="169"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="151"/>
+      <c r="F35" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="116" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="J35" s="29"/>
+      <c r="K35" s="107"/>
+    </row>
+    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="173"/>
+      <c r="B36" s="169"/>
+      <c r="C36" s="164"/>
+      <c r="D36" s="167"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="106" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="J36" s="29"/>
+      <c r="K36" s="107"/>
+    </row>
+    <row r="37" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="173"/>
+      <c r="B37" s="169"/>
+      <c r="C37" s="164"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="151"/>
+      <c r="F37" s="106" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J37" s="29"/>
+      <c r="K37" s="107"/>
+    </row>
+    <row r="38" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="173"/>
+      <c r="B38" s="169"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="167"/>
+      <c r="E38" s="151"/>
+      <c r="F38" s="106" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="116" t="s">
+        <v>104</v>
+      </c>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38" s="29"/>
+      <c r="K38" s="107"/>
+    </row>
+    <row r="39" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="174"/>
+      <c r="B39" s="170"/>
+      <c r="C39" s="165"/>
+      <c r="D39" s="168"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="117" t="s">
+        <v>106</v>
+      </c>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="J39" s="27"/>
+      <c r="K39" s="109"/>
+    </row>
+    <row r="40" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="172">
+        <v>5</v>
+      </c>
+      <c r="B40" s="171" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="163">
+        <v>5</v>
+      </c>
+      <c r="D40" s="166" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="150"/>
+      <c r="F40" s="104" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40" s="115" t="s">
+        <v>111</v>
+      </c>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="105"/>
+    </row>
+    <row r="41" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="173"/>
+      <c r="B41" s="169"/>
+      <c r="C41" s="164"/>
+      <c r="D41" s="167"/>
+      <c r="E41" s="151"/>
+      <c r="F41" s="106" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41" s="116" t="s">
+        <v>113</v>
+      </c>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="107"/>
+    </row>
+    <row r="42" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="173"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="167"/>
+      <c r="E42" s="151"/>
+      <c r="F42" s="106" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="116" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="J42" s="29"/>
+      <c r="K42" s="107"/>
+    </row>
+    <row r="43" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="173"/>
+      <c r="B43" s="169"/>
+      <c r="C43" s="164"/>
+      <c r="D43" s="167"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="106" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="J43" s="29"/>
+      <c r="K43" s="107"/>
+    </row>
+    <row r="44" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="174"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="165"/>
+      <c r="D44" s="168"/>
+      <c r="E44" s="152"/>
+      <c r="F44" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" s="117" t="s">
+        <v>121</v>
+      </c>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="J44" s="27"/>
+      <c r="K44" s="109"/>
+    </row>
+    <row r="45" spans="1:11" ht="39.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="99">
+        <v>6</v>
+      </c>
+      <c r="B45" s="100" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="101">
+        <v>1</v>
+      </c>
+      <c r="D45" s="110" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="110"/>
+      <c r="F45" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="119" t="s">
+        <v>125</v>
+      </c>
+      <c r="H45" s="102"/>
+      <c r="I45" s="131" t="s">
+        <v>126</v>
+      </c>
+      <c r="J45" s="28"/>
+      <c r="K45" s="103"/>
+    </row>
+    <row r="46" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="173">
+        <v>7</v>
+      </c>
+      <c r="B46" s="169" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="164">
+        <v>5</v>
+      </c>
+      <c r="D46" s="167" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="151"/>
+      <c r="F46" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="G46" s="115" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="105"/>
+    </row>
+    <row r="47" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="173"/>
+      <c r="B47" s="169"/>
+      <c r="C47" s="164"/>
+      <c r="D47" s="167"/>
+      <c r="E47" s="151"/>
+      <c r="F47" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G47" s="116" t="s">
+        <v>131</v>
+      </c>
+      <c r="H47" s="113"/>
+      <c r="I47" s="113"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="107"/>
+    </row>
+    <row r="48" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="173"/>
+      <c r="B48" s="169"/>
+      <c r="C48" s="164"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="151"/>
+      <c r="F48" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G48" s="116" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" s="113"/>
+      <c r="I48" s="113"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="107"/>
+    </row>
+    <row r="49" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="173"/>
+      <c r="B49" s="169"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="167"/>
+      <c r="E49" s="151"/>
+      <c r="F49" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G49" s="116" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" s="113"/>
+      <c r="I49" s="113"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="107"/>
+    </row>
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="174"/>
+      <c r="B50" s="170"/>
+      <c r="C50" s="165"/>
+      <c r="D50" s="168"/>
+      <c r="E50" s="152"/>
+      <c r="F50" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="G50" s="149" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="114"/>
+      <c r="I50" s="114"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="109"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J51" s="35"/>
+      <c r="K51" s="50"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F52" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F53" s="18"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F54" s="18"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="A9:A23"/>
+    <mergeCell ref="B9:B23"/>
+    <mergeCell ref="C9:C23"/>
+    <mergeCell ref="D9:D23"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="B24:B33"/>
+    <mergeCell ref="C24:C33"/>
+    <mergeCell ref="D24:D33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="D46:D50"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="J2:J16 J18:J50">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J16 J18:J50">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J16 J18:J50">
+      <formula1>"Passed, Failed, Blocked, Skipped"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007916DAE6CBAB0E478E10A9FCA3CC0E19" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc4eab9cdd79106b7ff0c84dd396c527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73b10483-4eab-47d9-97c6-997f49bd58aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c952eea70f5f85d64c583e57f778f77" ns2:_="">
     <xsd:import namespace="73b10483-4eab-47d9-97c6-997f49bd58aa"/>
@@ -7782,21 +9027,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4D3485E-123B-42CD-A17B-4E9A5EAAA4CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9450370A-E33A-4CBB-AE2E-AE21EC2991DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7814,11 +9060,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5589AC8F-1D80-4A3C-B04F-4E3B731AFF63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4D3485E-123B-42CD-A17B-4E9A5EAAA4CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>